<commit_message>
Fixed problem where storage root N was under leaf leaf appearance data
</commit_message>
<xml_diff>
--- a/Prototypes/FodderBeet/0bserved.xlsx
+++ b/Prototypes/FodderBeet/0bserved.xlsx
@@ -1194,10 +1194,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO1776"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1716" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BM1" sqref="BM1"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomLeft" activeCell="M1729" sqref="M1729:M1776"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84565,7 +84565,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="1729" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1729" s="1" t="s">
         <v>101</v>
       </c>
@@ -84587,9 +84587,6 @@
       <c r="H1729" s="4">
         <v>2.8228435657572302</v>
       </c>
-      <c r="I1729" s="4">
-        <v>6.5148295348857248</v>
-      </c>
       <c r="J1729" s="4">
         <v>13.80669450592276</v>
       </c>
@@ -84599,8 +84596,11 @@
       <c r="L1729" s="4">
         <v>1.4757162416485043</v>
       </c>
-    </row>
-    <row r="1730" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1729" s="4">
+        <v>6.5148295348857248</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1730" s="1" t="s">
         <v>101</v>
       </c>
@@ -84622,9 +84622,6 @@
       <c r="H1730" s="4">
         <v>3.2398836839611214</v>
       </c>
-      <c r="I1730" s="4">
-        <v>10.509027651304409</v>
-      </c>
       <c r="J1730" s="4">
         <v>18.164554735852569</v>
       </c>
@@ -84634,8 +84631,11 @@
       <c r="L1730" s="4">
         <v>1.6480475761396023</v>
       </c>
-    </row>
-    <row r="1731" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1730" s="4">
+        <v>10.509027651304409</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1731" s="1" t="s">
         <v>101</v>
       </c>
@@ -84657,9 +84657,6 @@
       <c r="H1731" s="4">
         <v>2.3004747854177228</v>
       </c>
-      <c r="I1731" s="4">
-        <v>16.548569713594915</v>
-      </c>
       <c r="J1731" s="4">
         <v>23.924075595656731</v>
       </c>
@@ -84669,8 +84666,11 @@
       <c r="L1731" s="4">
         <v>1.7753765345566594</v>
       </c>
-    </row>
-    <row r="1732" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1731" s="4">
+        <v>16.548569713594915</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1732" s="1" t="s">
         <v>102</v>
       </c>
@@ -84692,9 +84692,6 @@
       <c r="H1732" s="4">
         <v>3.790953865138825</v>
       </c>
-      <c r="I1732" s="4">
-        <v>9.6228158625089346</v>
-      </c>
       <c r="J1732" s="4">
         <v>21.270475784141908</v>
       </c>
@@ -84704,8 +84701,11 @@
       <c r="L1732" s="4">
         <v>2.7165561397281759</v>
       </c>
-    </row>
-    <row r="1733" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1732" s="4">
+        <v>9.6228158625089346</v>
+      </c>
+    </row>
+    <row r="1733" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1733" s="1" t="s">
         <v>102</v>
       </c>
@@ -84727,9 +84727,6 @@
       <c r="H1733" s="4">
         <v>4.2021028589468123</v>
       </c>
-      <c r="I1733" s="4">
-        <v>15.983756920012183</v>
-      </c>
       <c r="J1733" s="4">
         <v>26.66045039624667</v>
       </c>
@@ -84739,8 +84736,11 @@
       <c r="L1733" s="4">
         <v>2.9439698932141551</v>
       </c>
-    </row>
-    <row r="1734" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1733" s="4">
+        <v>15.983756920012183</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1734" s="1" t="s">
         <v>102</v>
       </c>
@@ -84762,9 +84762,6 @@
       <c r="H1734" s="4">
         <v>2.5693692362750573</v>
       </c>
-      <c r="I1734" s="4">
-        <v>21.164325926049006</v>
-      </c>
       <c r="J1734" s="4">
         <v>31.811266757972316</v>
       </c>
@@ -84774,8 +84771,11 @@
       <c r="L1734" s="4">
         <v>3.0234716384788385</v>
       </c>
-    </row>
-    <row r="1735" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1734" s="4">
+        <v>21.164325926049006</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1735" s="1" t="s">
         <v>103</v>
       </c>
@@ -84797,9 +84797,6 @@
       <c r="H1735" s="4">
         <v>4.0708349460401179</v>
       </c>
-      <c r="I1735" s="4">
-        <v>13.020268647521316</v>
-      </c>
       <c r="J1735" s="4">
         <v>26.059816253266337</v>
       </c>
@@ -84809,8 +84806,11 @@
       <c r="L1735" s="4">
         <v>3.2324040173912487</v>
       </c>
-    </row>
-    <row r="1736" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1735" s="4">
+        <v>13.020268647521316</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1736" s="1" t="s">
         <v>103</v>
       </c>
@@ -84832,9 +84832,6 @@
       <c r="H1736" s="4">
         <v>4.4364897529616014</v>
       </c>
-      <c r="I1736" s="4">
-        <v>21.362617370709234</v>
-      </c>
       <c r="J1736" s="4">
         <v>37.679936751457873</v>
       </c>
@@ -84844,8 +84841,11 @@
       <c r="L1736" s="4">
         <v>4.9356330791881673</v>
       </c>
-    </row>
-    <row r="1737" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1736" s="4">
+        <v>21.362617370709234</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1737" s="1" t="s">
         <v>103</v>
       </c>
@@ -84867,9 +84867,6 @@
       <c r="H1737" s="4">
         <v>2.7172307997430494</v>
       </c>
-      <c r="I1737" s="4">
-        <v>27.900349543913894</v>
-      </c>
       <c r="J1737" s="4">
         <v>38.316365502314255</v>
       </c>
@@ -84879,8 +84876,11 @@
       <c r="L1737" s="4">
         <v>3.0996850685279953</v>
       </c>
-    </row>
-    <row r="1738" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1737" s="4">
+        <v>27.900349543913894</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1738" s="1" t="s">
         <v>104</v>
       </c>
@@ -84902,9 +84902,6 @@
       <c r="H1738" s="4">
         <v>4.2290060338257556</v>
       </c>
-      <c r="I1738" s="4">
-        <v>12.443075154269231</v>
-      </c>
       <c r="J1738" s="4">
         <v>32.478090071288833</v>
       </c>
@@ -84914,8 +84911,11 @@
       <c r="L1738" s="4">
         <v>5.9730231516330994</v>
       </c>
-    </row>
-    <row r="1739" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1738" s="4">
+        <v>12.443075154269231</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1739" s="1" t="s">
         <v>104</v>
       </c>
@@ -84937,9 +84937,6 @@
       <c r="H1739" s="4">
         <v>4.2560523599076943</v>
       </c>
-      <c r="I1739" s="4">
-        <v>22.127618225270702</v>
-      </c>
       <c r="J1739" s="4">
         <v>39.108913797119449</v>
       </c>
@@ -84949,8 +84946,11 @@
       <c r="L1739" s="4">
         <v>5.5250428882956921</v>
       </c>
-    </row>
-    <row r="1740" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1739" s="4">
+        <v>22.127618225270702</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1740" s="1" t="s">
         <v>104</v>
       </c>
@@ -84972,9 +84972,6 @@
       <c r="H1740" s="4">
         <v>2.8111397554902187</v>
       </c>
-      <c r="I1740" s="4">
-        <v>40.694098916830129</v>
-      </c>
       <c r="J1740" s="4">
         <v>53.060803335599545</v>
       </c>
@@ -84984,8 +84981,11 @@
       <c r="L1740" s="4">
         <v>4.3762057738398621</v>
       </c>
-    </row>
-    <row r="1741" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1740" s="4">
+        <v>40.694098916830129</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1741" s="1" t="s">
         <v>105</v>
       </c>
@@ -85007,9 +85007,6 @@
       <c r="H1741" s="4">
         <v>2.8228435657572302</v>
       </c>
-      <c r="I1741" s="4">
-        <v>6.5148295348857248</v>
-      </c>
       <c r="J1741" s="4">
         <v>13.80669450592276</v>
       </c>
@@ -85019,8 +85016,11 @@
       <c r="L1741" s="4">
         <v>1.4757162416485043</v>
       </c>
-    </row>
-    <row r="1742" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1741" s="4">
+        <v>6.5148295348857248</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1742" s="1" t="s">
         <v>105</v>
       </c>
@@ -85042,9 +85042,6 @@
       <c r="H1742" s="4">
         <v>3.2398836839611214</v>
       </c>
-      <c r="I1742" s="4">
-        <v>10.509027651304409</v>
-      </c>
       <c r="J1742" s="4">
         <v>18.164554735852569</v>
       </c>
@@ -85054,8 +85051,11 @@
       <c r="L1742" s="4">
         <v>1.6480475761396023</v>
       </c>
-    </row>
-    <row r="1743" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1742" s="4">
+        <v>10.509027651304409</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1743" s="1" t="s">
         <v>105</v>
       </c>
@@ -85077,9 +85077,6 @@
       <c r="H1743" s="4">
         <v>2.3004747854177228</v>
       </c>
-      <c r="I1743" s="4">
-        <v>16.548569713594915</v>
-      </c>
       <c r="J1743" s="4">
         <v>23.924075595656731</v>
       </c>
@@ -85089,8 +85086,11 @@
       <c r="L1743" s="4">
         <v>1.7753765345566594</v>
       </c>
-    </row>
-    <row r="1744" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1743" s="4">
+        <v>16.548569713594915</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1744" s="1" t="s">
         <v>106</v>
       </c>
@@ -85112,9 +85112,6 @@
       <c r="H1744" s="4">
         <v>3.6183815226245724</v>
       </c>
-      <c r="I1744" s="4">
-        <v>8.3495094640190803</v>
-      </c>
       <c r="J1744" s="4">
         <v>17.985015015769395</v>
       </c>
@@ -85124,8 +85121,11 @@
       <c r="L1744" s="4">
         <v>2.1792004199614885</v>
       </c>
-    </row>
-    <row r="1745" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1744" s="4">
+        <v>8.3495094640190803</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1745" s="1" t="s">
         <v>106</v>
       </c>
@@ -85147,9 +85147,6 @@
       <c r="H1745" s="4">
         <v>3.9080490512188164</v>
       </c>
-      <c r="I1745" s="4">
-        <v>11.678343418710993</v>
-      </c>
       <c r="J1745" s="4">
         <v>21.911235811271034</v>
       </c>
@@ -85159,8 +85156,11 @@
       <c r="L1745" s="4">
         <v>2.8999558769283174</v>
       </c>
-    </row>
-    <row r="1746" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1745" s="4">
+        <v>11.678343418710993</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1746" s="1" t="s">
         <v>106</v>
       </c>
@@ -85182,9 +85182,6 @@
       <c r="H1746" s="4">
         <v>2.4974428718926771</v>
       </c>
-      <c r="I1746" s="4">
-        <v>21.283610070094742</v>
-      </c>
       <c r="J1746" s="4">
         <v>31.246972155249484</v>
       </c>
@@ -85194,8 +85191,11 @@
       <c r="L1746" s="4">
         <v>2.8069774407555572</v>
       </c>
-    </row>
-    <row r="1747" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1746" s="4">
+        <v>21.283610070094742</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1747" s="1" t="s">
         <v>107</v>
       </c>
@@ -85217,9 +85217,6 @@
       <c r="H1747" s="4">
         <v>4.4233469550379203</v>
       </c>
-      <c r="I1747" s="4">
-        <v>10.57965266349248</v>
-      </c>
       <c r="J1747" s="4">
         <v>23.864158296484685</v>
       </c>
@@ -85229,8 +85226,11 @@
       <c r="L1747" s="4">
         <v>2.8088540960679622</v>
       </c>
-    </row>
-    <row r="1748" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1747" s="4">
+        <v>10.57965266349248</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1748" s="1" t="s">
         <v>107</v>
       </c>
@@ -85252,9 +85252,6 @@
       <c r="H1748" s="4">
         <v>4.1143825460886854</v>
       </c>
-      <c r="I1748" s="4">
-        <v>15.752970366620705</v>
-      </c>
       <c r="J1748" s="4">
         <v>28.961911247073385</v>
       </c>
@@ -85264,8 +85261,11 @@
       <c r="L1748" s="4">
         <v>3.5009221410635618</v>
       </c>
-    </row>
-    <row r="1749" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1748" s="4">
+        <v>15.752970366620705</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1749" s="1" t="s">
         <v>107</v>
       </c>
@@ -85287,9 +85287,6 @@
       <c r="H1749" s="4">
         <v>2.4742409421720422</v>
       </c>
-      <c r="I1749" s="4">
-        <v>31.15411282631738</v>
-      </c>
       <c r="J1749" s="4">
         <v>43.029748838355765</v>
       </c>
@@ -85299,8 +85296,11 @@
       <c r="L1749" s="4">
         <v>3.7679354650874535</v>
       </c>
-    </row>
-    <row r="1750" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1749" s="4">
+        <v>31.15411282631738</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1750" s="1" t="s">
         <v>108</v>
       </c>
@@ -85322,9 +85322,6 @@
       <c r="H1750" s="4">
         <v>2.9010304756876182</v>
       </c>
-      <c r="I1750" s="4">
-        <v>7.4277299202587006</v>
-      </c>
       <c r="J1750" s="4">
         <v>16.667412048785096</v>
       </c>
@@ -85334,8 +85331,11 @@
       <c r="L1750" s="4">
         <v>2.0829418250950793</v>
       </c>
-    </row>
-    <row r="1751" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1750" s="4">
+        <v>7.4277299202587006</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1751" s="1" t="s">
         <v>108</v>
       </c>
@@ -85357,9 +85357,6 @@
       <c r="H1751" s="4">
         <v>4.7737215368756845</v>
       </c>
-      <c r="I1751" s="4">
-        <v>16.975057797244997</v>
-      </c>
       <c r="J1751" s="4">
         <v>33.152961531383276</v>
       </c>
@@ -85369,8 +85366,11 @@
       <c r="L1751" s="4">
         <v>4.7567890299091236</v>
       </c>
-    </row>
-    <row r="1752" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1751" s="4">
+        <v>16.975057797244997</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1752" s="1" t="s">
         <v>108</v>
       </c>
@@ -85392,9 +85392,6 @@
       <c r="H1752" s="4">
         <v>2.8632184941481178</v>
       </c>
-      <c r="I1752" s="4">
-        <v>31.356314164805116</v>
-      </c>
       <c r="J1752" s="4">
         <v>44.751008534468518</v>
       </c>
@@ -85404,8 +85401,11 @@
       <c r="L1752" s="4">
         <v>4.0356093262641366</v>
       </c>
-    </row>
-    <row r="1753" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1752" s="4">
+        <v>31.356314164805116</v>
+      </c>
+    </row>
+    <row r="1753" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1753" s="1" t="s">
         <v>109</v>
       </c>
@@ -85427,9 +85427,6 @@
       <c r="H1753" s="4">
         <v>3.7814364084808609</v>
       </c>
-      <c r="I1753" s="4">
-        <v>5.0691727186625943</v>
-      </c>
       <c r="J1753" s="4">
         <v>13.815443929649907</v>
       </c>
@@ -85439,8 +85436,11 @@
       <c r="L1753" s="4">
         <v>1.9766891920118339</v>
       </c>
-    </row>
-    <row r="1754" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1753" s="4">
+        <v>5.0691727186625943</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1754" s="1" t="s">
         <v>109</v>
       </c>
@@ -85462,9 +85462,6 @@
       <c r="H1754" s="4">
         <v>2.2682886732193741</v>
       </c>
-      <c r="I1754" s="4">
-        <v>7.5728562056851745</v>
-      </c>
       <c r="J1754" s="4">
         <v>12.41678859348584</v>
       </c>
@@ -85474,8 +85471,11 @@
       <c r="L1754" s="4">
         <v>0.99484720152533812</v>
       </c>
-    </row>
-    <row r="1755" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1754" s="4">
+        <v>7.5728562056851745</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1755" s="1" t="s">
         <v>109</v>
       </c>
@@ -85497,9 +85497,6 @@
       <c r="H1755" s="4">
         <v>1.6272920943265492</v>
       </c>
-      <c r="I1755" s="4">
-        <v>10.401278471708364</v>
-      </c>
       <c r="J1755" s="4">
         <v>15.967449943501638</v>
       </c>
@@ -85509,8 +85506,11 @@
       <c r="L1755" s="4">
         <v>1.5460128435507423</v>
       </c>
-    </row>
-    <row r="1756" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1755" s="4">
+        <v>10.401278471708364</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1756" s="1" t="s">
         <v>110</v>
       </c>
@@ -85532,9 +85532,6 @@
       <c r="H1756" s="4">
         <v>4.6052429635158258</v>
       </c>
-      <c r="I1756" s="4">
-        <v>9.2150360649040071</v>
-      </c>
       <c r="J1756" s="4">
         <v>20.813562118941853</v>
       </c>
@@ -85544,8 +85541,11 @@
       <c r="L1756" s="4">
         <v>3.0432790697601444</v>
       </c>
-    </row>
-    <row r="1757" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1756" s="4">
+        <v>9.2150360649040071</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1757" s="1" t="s">
         <v>110</v>
       </c>
@@ -85567,9 +85567,6 @@
       <c r="H1757" s="4">
         <v>2.5890212703571129</v>
       </c>
-      <c r="I1757" s="4">
-        <v>6.1407926036029288</v>
-      </c>
       <c r="J1757" s="4">
         <v>19.13109591127267</v>
       </c>
@@ -85579,8 +85576,11 @@
       <c r="L1757" s="4">
         <v>3.6157898238826371</v>
       </c>
-    </row>
-    <row r="1758" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1757" s="4">
+        <v>6.1407926036029288</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1758" s="1" t="s">
         <v>110</v>
       </c>
@@ -85602,9 +85602,6 @@
       <c r="H1758" s="4">
         <v>1.6979032687290545</v>
       </c>
-      <c r="I1758" s="4">
-        <v>9.9854686102027621</v>
-      </c>
       <c r="J1758" s="4">
         <v>17.369605121290967</v>
       </c>
@@ -85614,8 +85611,11 @@
       <c r="L1758" s="4">
         <v>1.7373055657073635</v>
       </c>
-    </row>
-    <row r="1759" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1758" s="4">
+        <v>9.9854686102027621</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1759" s="1" t="s">
         <v>111</v>
       </c>
@@ -85637,9 +85637,6 @@
       <c r="H1759" s="4">
         <v>3.5832439569853247</v>
       </c>
-      <c r="I1759" s="4">
-        <v>13.90387093430331</v>
-      </c>
       <c r="J1759" s="4">
         <v>19.50857429187738</v>
       </c>
@@ -85649,8 +85646,11 @@
       <c r="L1759" s="4">
         <v>1.5719074635341479</v>
       </c>
-    </row>
-    <row r="1760" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1759" s="4">
+        <v>13.90387093430331</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1760" s="1" t="s">
         <v>111</v>
       </c>
@@ -85672,9 +85672,6 @@
       <c r="H1760" s="4">
         <v>4.262579744534241</v>
       </c>
-      <c r="I1760" s="4">
-        <v>17.901985097826739</v>
-      </c>
       <c r="J1760" s="4">
         <v>32.766475242998609</v>
       </c>
@@ -85684,8 +85681,11 @@
       <c r="L1760" s="4">
         <v>4.3735599672944669</v>
       </c>
-    </row>
-    <row r="1761" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1760" s="4">
+        <v>17.901985097826739</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1761" s="1" t="s">
         <v>111</v>
       </c>
@@ -85707,9 +85707,6 @@
       <c r="H1761" s="4">
         <v>2.2723189443961092</v>
       </c>
-      <c r="I1761" s="4">
-        <v>22.833554478233008</v>
-      </c>
       <c r="J1761" s="4">
         <v>34.324623460399508</v>
       </c>
@@ -85719,8 +85716,11 @@
       <c r="L1761" s="4">
         <v>3.6315082460778507</v>
       </c>
-    </row>
-    <row r="1762" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1761" s="4">
+        <v>22.833554478233008</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1762" s="1" t="s">
         <v>112</v>
       </c>
@@ -85742,9 +85742,6 @@
       <c r="H1762" s="4">
         <v>5.0265268732837702</v>
       </c>
-      <c r="I1762" s="4">
-        <v>12.603324723228241</v>
-      </c>
       <c r="J1762" s="4">
         <v>29.800825811730739</v>
       </c>
@@ -85754,8 +85751,11 @@
       <c r="L1762" s="4">
         <v>5.3867781607166823</v>
       </c>
-    </row>
-    <row r="1763" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1762" s="4">
+        <v>12.603324723228241</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1763" s="1" t="s">
         <v>112</v>
       </c>
@@ -85777,9 +85777,6 @@
       <c r="H1763" s="4">
         <v>4.1528409101900916</v>
       </c>
-      <c r="I1763" s="4">
-        <v>16.349645571337202</v>
-      </c>
       <c r="J1763" s="4">
         <v>31.446737210672456</v>
       </c>
@@ -85789,8 +85786,11 @@
       <c r="L1763" s="4">
         <v>4.4848939664859264</v>
       </c>
-    </row>
-    <row r="1764" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1763" s="4">
+        <v>16.349645571337202</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1764" s="1" t="s">
         <v>112</v>
       </c>
@@ -85812,9 +85812,6 @@
       <c r="H1764" s="4">
         <v>2.5994842985592084</v>
       </c>
-      <c r="I1764" s="4">
-        <v>26.364796988607754</v>
-      </c>
       <c r="J1764" s="4">
         <v>37.540272432551021</v>
       </c>
@@ -85824,8 +85821,11 @@
       <c r="L1764" s="4">
         <v>3.4459470949265145</v>
       </c>
-    </row>
-    <row r="1765" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1764" s="4">
+        <v>26.364796988607754</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1765" s="1" t="s">
         <v>113</v>
       </c>
@@ -85847,9 +85847,6 @@
       <c r="H1765" s="4">
         <v>3.7814364084808609</v>
       </c>
-      <c r="I1765" s="4">
-        <v>5.0691727186625943</v>
-      </c>
       <c r="J1765" s="4">
         <v>13.815443929649907</v>
       </c>
@@ -85859,8 +85856,11 @@
       <c r="L1765" s="4">
         <v>1.9766891920118339</v>
       </c>
-    </row>
-    <row r="1766" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1765" s="4">
+        <v>5.0691727186625943</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1766" s="1" t="s">
         <v>113</v>
       </c>
@@ -85882,9 +85882,6 @@
       <c r="H1766" s="4">
         <v>2.2682886732193741</v>
       </c>
-      <c r="I1766" s="4">
-        <v>7.5728562056851745</v>
-      </c>
       <c r="J1766" s="4">
         <v>12.41678859348584</v>
       </c>
@@ -85894,8 +85891,11 @@
       <c r="L1766" s="4">
         <v>0.99484720152533812</v>
       </c>
-    </row>
-    <row r="1767" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1766" s="4">
+        <v>7.5728562056851745</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1767" s="1" t="s">
         <v>113</v>
       </c>
@@ -85917,9 +85917,6 @@
       <c r="H1767" s="4">
         <v>1.6272920943265492</v>
       </c>
-      <c r="I1767" s="4">
-        <v>10.401278471708364</v>
-      </c>
       <c r="J1767" s="4">
         <v>15.967449943501638</v>
       </c>
@@ -85929,8 +85926,11 @@
       <c r="L1767" s="4">
         <v>1.5460128435507423</v>
       </c>
-    </row>
-    <row r="1768" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1767" s="4">
+        <v>10.401278471708364</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1768" s="1" t="s">
         <v>114</v>
       </c>
@@ -85952,9 +85952,6 @@
       <c r="H1768" s="4">
         <v>3.9807145601239422</v>
       </c>
-      <c r="I1768" s="4">
-        <v>6.4631287750204551</v>
-      </c>
       <c r="J1768" s="4">
         <v>15.744767978098967</v>
       </c>
@@ -85964,8 +85961,11 @@
       <c r="L1768" s="4">
         <v>2.1781985094356244</v>
       </c>
-    </row>
-    <row r="1769" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1768" s="4">
+        <v>6.4631287750204551</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1769" s="1" t="s">
         <v>114</v>
       </c>
@@ -85987,9 +85987,6 @@
       <c r="H1769" s="4">
         <v>2.7032883533303824</v>
       </c>
-      <c r="I1769" s="4">
-        <v>8.9517239877050603</v>
-      </c>
       <c r="J1769" s="4">
         <v>15.061213877843297</v>
       </c>
@@ -85999,8 +85996,11 @@
       <c r="L1769" s="4">
         <v>1.5203089107762442</v>
       </c>
-    </row>
-    <row r="1770" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1769" s="4">
+        <v>8.9517239877050603</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1770" s="1" t="s">
         <v>114</v>
       </c>
@@ -86022,9 +86022,6 @@
       <c r="H1770" s="4">
         <v>1.6299918523231671</v>
       </c>
-      <c r="I1770" s="4">
-        <v>16.167319060149257</v>
-      </c>
       <c r="J1770" s="4">
         <v>23.033196327095798</v>
       </c>
@@ -86034,8 +86031,11 @@
       <c r="L1770" s="4">
         <v>1.6723251781528976</v>
       </c>
-    </row>
-    <row r="1771" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1770" s="4">
+        <v>16.167319060149257</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1771" s="1" t="s">
         <v>115</v>
       </c>
@@ -86057,9 +86057,6 @@
       <c r="H1771" s="4">
         <v>4.0642713605075587</v>
       </c>
-      <c r="I1771" s="4">
-        <v>6.4993072837469921</v>
-      </c>
       <c r="J1771" s="4">
         <v>16.695747760539234</v>
       </c>
@@ -86069,8 +86066,11 @@
       <c r="L1771" s="4">
         <v>2.1777057267351125</v>
       </c>
-    </row>
-    <row r="1772" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1771" s="4">
+        <v>6.4993072837469921</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1772" s="1" t="s">
         <v>115</v>
       </c>
@@ -86092,9 +86092,6 @@
       <c r="H1772" s="4">
         <v>3.2145307349560199</v>
       </c>
-      <c r="I1772" s="4">
-        <v>11.706549203309685</v>
-      </c>
       <c r="J1772" s="4">
         <v>19.736380195215602</v>
       </c>
@@ -86104,8 +86101,11 @@
       <c r="L1772" s="4">
         <v>1.9103330899969706</v>
       </c>
-    </row>
-    <row r="1773" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1772" s="4">
+        <v>11.706549203309685</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1773" s="1" t="s">
         <v>115</v>
       </c>
@@ -86127,9 +86127,6 @@
       <c r="H1773" s="4">
         <v>2.6494412206119797</v>
       </c>
-      <c r="I1773" s="4">
-        <v>22.910745503604936</v>
-      </c>
       <c r="J1773" s="4">
         <v>33.343635614813678</v>
       </c>
@@ -86139,8 +86136,11 @@
       <c r="L1773" s="4">
         <v>2.8593773189663079</v>
       </c>
-    </row>
-    <row r="1774" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1773" s="4">
+        <v>22.910745503604936</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1774" s="1" t="s">
         <v>116</v>
       </c>
@@ -86162,9 +86162,6 @@
       <c r="H1774" s="4">
         <v>3.4996024579268421</v>
       </c>
-      <c r="I1774" s="4">
-        <v>8.0716651119090486</v>
-      </c>
       <c r="J1774" s="4">
         <v>18.667315565669803</v>
       </c>
@@ -86174,8 +86171,11 @@
       <c r="L1774" s="4">
         <v>2.2578217113912928</v>
       </c>
-    </row>
-    <row r="1775" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1774" s="4">
+        <v>8.0716651119090486</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1775" s="1" t="s">
         <v>116</v>
       </c>
@@ -86197,9 +86197,6 @@
       <c r="H1775" s="4">
         <v>4.0494601857434303</v>
       </c>
-      <c r="I1775" s="4">
-        <v>16.872965895752735</v>
-      </c>
       <c r="J1775" s="4">
         <v>29.817393550030744</v>
       </c>
@@ -86209,8 +86206,11 @@
       <c r="L1775" s="4">
         <v>3.2988681591590066</v>
       </c>
-    </row>
-    <row r="1776" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1775" s="4">
+        <v>16.872965895752735</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1776" s="1" t="s">
         <v>116</v>
       </c>
@@ -86232,9 +86232,6 @@
       <c r="H1776" s="4">
         <v>2.7728082119859678</v>
       </c>
-      <c r="I1776" s="4">
-        <v>26.136583235171365</v>
-      </c>
       <c r="J1776" s="4">
         <v>38.831737446934753</v>
       </c>
@@ -86243,6 +86240,9 @@
       </c>
       <c r="L1776" s="4">
         <v>4.1279386322428815</v>
+      </c>
+      <c r="M1776" s="4">
+        <v>26.136583235171365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated observed file to include more SFF
</commit_message>
<xml_diff>
--- a/Prototypes/FodderBeet/0bserved.xlsx
+++ b/Prototypes/FodderBeet/0bserved.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3569" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="155">
   <si>
     <t>SimulationName</t>
   </si>
@@ -370,6 +370,120 @@
   </si>
   <si>
     <t>GoreNit300Splits3</t>
+  </si>
+  <si>
+    <t>RakaiaNit0Splits2</t>
+  </si>
+  <si>
+    <t>RakaiaNit100Splits2</t>
+  </si>
+  <si>
+    <t>RakaiaNit200Splits2</t>
+  </si>
+  <si>
+    <t>RakaiaNit300Splits2</t>
+  </si>
+  <si>
+    <t>RakaiaNit0Splits3</t>
+  </si>
+  <si>
+    <t>RakaiaNit100Splits3</t>
+  </si>
+  <si>
+    <t>RakaiaNit200Splits3</t>
+  </si>
+  <si>
+    <t>RakaiaNit300Splits3</t>
+  </si>
+  <si>
+    <t>RivertonNit0Splits2</t>
+  </si>
+  <si>
+    <t>RivertonNit100Splits2</t>
+  </si>
+  <si>
+    <t>RivertonNit200Splits2</t>
+  </si>
+  <si>
+    <t>RivertonNit300Splits2</t>
+  </si>
+  <si>
+    <t>RivertonNit0Splits3</t>
+  </si>
+  <si>
+    <t>RivertonNit100Splits3</t>
+  </si>
+  <si>
+    <t>RivertonNit200Splits3</t>
+  </si>
+  <si>
+    <t>RivertonNit300Splits3</t>
+  </si>
+  <si>
+    <t>WhanganuiNit0Splits2</t>
+  </si>
+  <si>
+    <t>WhanganuiNit100Splits2</t>
+  </si>
+  <si>
+    <t>WhanganuiNit200Splits2</t>
+  </si>
+  <si>
+    <t>WhanganuiNit300Splits2</t>
+  </si>
+  <si>
+    <t>WhanganuiNit0Splits3</t>
+  </si>
+  <si>
+    <t>WhanganuiNit100Splits3</t>
+  </si>
+  <si>
+    <t>WhanganuiNit200Splits3</t>
+  </si>
+  <si>
+    <t>WhanganuiNit300Splits3</t>
+  </si>
+  <si>
+    <t>TaranakiNit0Splits2</t>
+  </si>
+  <si>
+    <t>TaranakiNit100Splits2</t>
+  </si>
+  <si>
+    <t>TaranakiNit200Splits2</t>
+  </si>
+  <si>
+    <t>TaranakiNit300Splits2</t>
+  </si>
+  <si>
+    <t>TaranakiNit100Splits3</t>
+  </si>
+  <si>
+    <t>TaranakiNit200Splits3</t>
+  </si>
+  <si>
+    <t>TaranakiNit300Splits3</t>
+  </si>
+  <si>
+    <t>WaikatoNit0Splits2</t>
+  </si>
+  <si>
+    <t>WaikatoNit100Splits2</t>
+  </si>
+  <si>
+    <t>WaikatoNit200Splits2</t>
+  </si>
+  <si>
+    <t>WaikatoNit300Splits2</t>
+  </si>
+  <si>
+    <t>WaikatoNit100Splits3</t>
+  </si>
+  <si>
+    <t>WaikatoNit200Splits3</t>
+  </si>
+  <si>
+    <t>WaikatoNit300Splits3</t>
   </si>
 </sst>
 </file>
@@ -857,7 +971,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -871,6 +985,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1192,12 +1311,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BO1776"/>
+  <dimension ref="A1:BO1888"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1716" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1806" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="BM1" sqref="BM1"/>
-      <selection pane="bottomLeft" activeCell="M1729" sqref="M1729:M1776"/>
+      <selection pane="bottomLeft" activeCell="C1786" sqref="C1786"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="34.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -86245,6 +86364,3926 @@
         <v>26.136583235171365</v>
       </c>
     </row>
+    <row r="1777" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1777" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1777" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1777" s="6">
+        <v>1466.3869276652215</v>
+      </c>
+      <c r="D1777" s="6">
+        <v>253.98030017185835</v>
+      </c>
+      <c r="E1777" s="6">
+        <v>218.21628139285727</v>
+      </c>
+      <c r="F1777" s="6">
+        <v>946.72148460116864</v>
+      </c>
+      <c r="H1777" s="6">
+        <v>2.6507758292528663</v>
+      </c>
+      <c r="J1777" s="6">
+        <v>20.969725573783869</v>
+      </c>
+      <c r="K1777" s="6">
+        <v>7.1810204810058753</v>
+      </c>
+      <c r="L1777" s="6">
+        <v>2.2592715778721142</v>
+      </c>
+      <c r="M1777" s="6">
+        <v>11.022367900714091</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1778" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1778" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1778" s="6">
+        <v>2125.1713283567669</v>
+      </c>
+      <c r="D1778" s="6">
+        <v>175.23227854682838</v>
+      </c>
+      <c r="E1778" s="6">
+        <v>203.11880372537556</v>
+      </c>
+      <c r="F1778" s="6">
+        <v>1690.0276626412863</v>
+      </c>
+      <c r="H1778" s="6">
+        <v>3.0911548966270375</v>
+      </c>
+      <c r="J1778" s="6">
+        <v>20.589045419504025</v>
+      </c>
+      <c r="K1778" s="6">
+        <v>5.3085550172896765</v>
+      </c>
+      <c r="L1778" s="6">
+        <v>1.9856405668118913</v>
+      </c>
+      <c r="M1778" s="6">
+        <v>12.813606672334757</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1779" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1779" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1779" s="6">
+        <v>2609.9160605172733</v>
+      </c>
+      <c r="D1779" s="6">
+        <v>109.45746634196568</v>
+      </c>
+      <c r="E1779" s="6">
+        <v>86.652563485525604</v>
+      </c>
+      <c r="F1779" s="6">
+        <v>2273.5455873976448</v>
+      </c>
+      <c r="H1779" s="6">
+        <v>1.6953310192883457</v>
+      </c>
+      <c r="J1779" s="6">
+        <v>25.123042750031519</v>
+      </c>
+      <c r="K1779" s="6">
+        <v>4.0106810405238145</v>
+      </c>
+      <c r="L1779" s="6">
+        <v>1.5803361050294387</v>
+      </c>
+      <c r="M1779" s="6">
+        <v>17.863228434364508</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1780" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1780" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1780" s="6">
+        <v>1277.1638698258078</v>
+      </c>
+      <c r="D1780" s="6">
+        <v>202.34441889828565</v>
+      </c>
+      <c r="E1780" s="6">
+        <v>208.5367441185675</v>
+      </c>
+      <c r="F1780" s="6">
+        <v>823.9979280638787</v>
+      </c>
+      <c r="H1780" s="6">
+        <v>3.3857754398728841</v>
+      </c>
+      <c r="J1780" s="6">
+        <v>18.773225483536756</v>
+      </c>
+      <c r="K1780" s="6">
+        <v>5.9622875159597974</v>
+      </c>
+      <c r="L1780" s="6">
+        <v>2.1458599945114614</v>
+      </c>
+      <c r="M1780" s="6">
+        <v>10.234679183979846</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1781" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1781" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1781" s="6">
+        <v>2154.850381224634</v>
+      </c>
+      <c r="D1781" s="6">
+        <v>195.42998821483005</v>
+      </c>
+      <c r="E1781" s="6">
+        <v>260.91734571900088</v>
+      </c>
+      <c r="F1781" s="6">
+        <v>1619.8806549699916</v>
+      </c>
+      <c r="H1781" s="6">
+        <v>3.6310511496324556</v>
+      </c>
+      <c r="J1781" s="6">
+        <v>25.036159496104336</v>
+      </c>
+      <c r="K1781" s="6">
+        <v>6.4576230810281618</v>
+      </c>
+      <c r="L1781" s="6">
+        <v>2.6485933440416392</v>
+      </c>
+      <c r="M1781" s="6">
+        <v>15.275509382572386</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1782" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1782" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1782" s="6">
+        <v>2706.8829727108023</v>
+      </c>
+      <c r="D1782" s="6">
+        <v>119.56169426519116</v>
+      </c>
+      <c r="E1782" s="6">
+        <v>80.06783583967686</v>
+      </c>
+      <c r="F1782" s="6">
+        <v>2342.4164294735019</v>
+      </c>
+      <c r="H1782" s="6">
+        <v>1.5805846319125578</v>
+      </c>
+      <c r="J1782" s="6">
+        <v>32.315507660373768</v>
+      </c>
+      <c r="K1782" s="6">
+        <v>4.3482411230444518</v>
+      </c>
+      <c r="L1782" s="6">
+        <v>1.6319038276147482</v>
+      </c>
+      <c r="M1782" s="6">
+        <v>24.20334982684648</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1783" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1783" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1783" s="6">
+        <v>1635.0231436143677</v>
+      </c>
+      <c r="D1783" s="6">
+        <v>293.67983688806123</v>
+      </c>
+      <c r="E1783" s="6">
+        <v>305.74202453528574</v>
+      </c>
+      <c r="F1783" s="6">
+        <v>974.95177161353877</v>
+      </c>
+      <c r="H1783" s="6">
+        <v>4.8677976427165524</v>
+      </c>
+      <c r="J1783" s="6">
+        <v>27.516467554348246</v>
+      </c>
+      <c r="K1783" s="6">
+        <v>9.2104377147740699</v>
+      </c>
+      <c r="L1783" s="6">
+        <v>3.967836751006562</v>
+      </c>
+      <c r="M1783" s="6">
+        <v>13.530805508927765</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1784" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1784" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1784" s="6">
+        <v>2092.569442111208</v>
+      </c>
+      <c r="D1784" s="6">
+        <v>226.66380828926472</v>
+      </c>
+      <c r="E1784" s="6">
+        <v>318.34013995361988</v>
+      </c>
+      <c r="F1784" s="6">
+        <v>1444.178050875121</v>
+      </c>
+      <c r="H1784" s="6">
+        <v>4.0024695339145664</v>
+      </c>
+      <c r="J1784" s="6">
+        <v>35.51701960615442</v>
+      </c>
+      <c r="K1784" s="6">
+        <v>8.3431319663425274</v>
+      </c>
+      <c r="L1784" s="6">
+        <v>4.2438725521366329</v>
+      </c>
+      <c r="M1784" s="6">
+        <v>21.806668086489449</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1785" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1785" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1785" s="6">
+        <v>2639.9050235028953</v>
+      </c>
+      <c r="D1785" s="6">
+        <v>105.91525086851804</v>
+      </c>
+      <c r="E1785" s="6">
+        <v>66.86774291932069</v>
+      </c>
+      <c r="F1785" s="6">
+        <v>2255.2520948182191</v>
+      </c>
+      <c r="H1785" s="6">
+        <v>1.5438238133663447</v>
+      </c>
+      <c r="J1785" s="6">
+        <v>38.939690439225188</v>
+      </c>
+      <c r="K1785" s="6">
+        <v>4.1527337782123368</v>
+      </c>
+      <c r="L1785" s="6">
+        <v>1.6014105153946609</v>
+      </c>
+      <c r="M1785" s="6">
+        <v>29.104634382894851</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1786" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1786" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1786" s="6">
+        <v>1602.6252548928192</v>
+      </c>
+      <c r="D1786" s="6">
+        <v>262.31880325636837</v>
+      </c>
+      <c r="E1786" s="6">
+        <v>285.66942464856004</v>
+      </c>
+      <c r="F1786" s="6">
+        <v>1007.0273057436704</v>
+      </c>
+      <c r="H1786" s="6">
+        <v>4.1643403285143092</v>
+      </c>
+      <c r="J1786" s="6">
+        <v>34.721412929982037</v>
+      </c>
+      <c r="K1786" s="6">
+        <v>10.164271873386758</v>
+      </c>
+      <c r="L1786" s="6">
+        <v>4.8567082301368369</v>
+      </c>
+      <c r="M1786" s="6">
+        <v>19.045967512618709</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1787" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1787" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1787" s="6">
+        <v>2336.8663714706386</v>
+      </c>
+      <c r="D1787" s="6">
+        <v>254.18328121472808</v>
+      </c>
+      <c r="E1787" s="6">
+        <v>329.27042863996286</v>
+      </c>
+      <c r="F1787" s="6">
+        <v>1700.1856829119074</v>
+      </c>
+      <c r="H1787" s="6">
+        <v>4.5178182206202928</v>
+      </c>
+      <c r="J1787" s="6">
+        <v>44.976399924979177</v>
+      </c>
+      <c r="K1787" s="6">
+        <v>11.176711558316786</v>
+      </c>
+      <c r="L1787" s="6">
+        <v>6.2705986290185365</v>
+      </c>
+      <c r="M1787" s="6">
+        <v>26.930405829558488</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1788" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1788" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1788" s="6">
+        <v>2578.6249790718402</v>
+      </c>
+      <c r="D1788" s="6">
+        <v>137.88038956981043</v>
+      </c>
+      <c r="E1788" s="6">
+        <v>98.809210144537388</v>
+      </c>
+      <c r="F1788" s="6">
+        <v>2194.3177983006308</v>
+      </c>
+      <c r="H1788" s="6">
+        <v>2.0699128340443678</v>
+      </c>
+      <c r="J1788" s="6">
+        <v>40.601277671493584</v>
+      </c>
+      <c r="K1788" s="6">
+        <v>5.3365790564809119</v>
+      </c>
+      <c r="L1788" s="6">
+        <v>2.339946838169392</v>
+      </c>
+      <c r="M1788" s="6">
+        <v>29.925020371880532</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1789" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1789" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1789" s="6">
+        <v>1466.3869276652215</v>
+      </c>
+      <c r="D1789" s="6">
+        <v>253.98030017185835</v>
+      </c>
+      <c r="E1789" s="6">
+        <v>218.21628139285727</v>
+      </c>
+      <c r="F1789" s="6">
+        <v>946.72148460116864</v>
+      </c>
+      <c r="H1789" s="6">
+        <v>2.6507758292528663</v>
+      </c>
+      <c r="J1789" s="6">
+        <v>20.969725573783869</v>
+      </c>
+      <c r="K1789" s="6">
+        <v>7.1810204810058753</v>
+      </c>
+      <c r="L1789" s="6">
+        <v>2.2592715778721142</v>
+      </c>
+      <c r="M1789" s="6">
+        <v>11.022367900714091</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1790" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1790" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1790" s="6">
+        <v>2125.1713283567669</v>
+      </c>
+      <c r="D1790" s="6">
+        <v>175.23227854682838</v>
+      </c>
+      <c r="E1790" s="6">
+        <v>203.11880372537556</v>
+      </c>
+      <c r="F1790" s="6">
+        <v>1690.0276626412863</v>
+      </c>
+      <c r="H1790" s="6">
+        <v>3.0911548966270375</v>
+      </c>
+      <c r="J1790" s="6">
+        <v>20.589045419504025</v>
+      </c>
+      <c r="K1790" s="6">
+        <v>5.3085550172896765</v>
+      </c>
+      <c r="L1790" s="6">
+        <v>1.9856405668118913</v>
+      </c>
+      <c r="M1790" s="6">
+        <v>12.813606672334757</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1791" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1791" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1791" s="6">
+        <v>2609.9160605172733</v>
+      </c>
+      <c r="D1791" s="6">
+        <v>109.45746634196568</v>
+      </c>
+      <c r="E1791" s="6">
+        <v>86.652563485525604</v>
+      </c>
+      <c r="F1791" s="6">
+        <v>2273.5455873976448</v>
+      </c>
+      <c r="H1791" s="6">
+        <v>1.6953310192883457</v>
+      </c>
+      <c r="J1791" s="6">
+        <v>25.123042750031519</v>
+      </c>
+      <c r="K1791" s="6">
+        <v>4.0106810405238145</v>
+      </c>
+      <c r="L1791" s="6">
+        <v>1.5803361050294387</v>
+      </c>
+      <c r="M1791" s="6">
+        <v>17.863228434364508</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1792" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1792" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1792" s="6">
+        <v>1298.3767721146955</v>
+      </c>
+      <c r="D1792" s="6">
+        <v>236.38221583609848</v>
+      </c>
+      <c r="E1792" s="6">
+        <v>222.19608890446975</v>
+      </c>
+      <c r="F1792" s="6">
+        <v>786.99143217788924</v>
+      </c>
+      <c r="H1792" s="6">
+        <v>3.8056654980386448</v>
+      </c>
+      <c r="J1792" s="6">
+        <v>21.344192817299657</v>
+      </c>
+      <c r="K1792" s="6">
+        <v>7.3214711142905742</v>
+      </c>
+      <c r="L1792" s="6">
+        <v>2.7008440615395219</v>
+      </c>
+      <c r="M1792" s="6">
+        <v>10.712290800594666</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1793" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1793" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1793" s="6">
+        <v>2142.8607746850748</v>
+      </c>
+      <c r="D1793" s="6">
+        <v>201.63539945790723</v>
+      </c>
+      <c r="E1793" s="6">
+        <v>272.56769872904619</v>
+      </c>
+      <c r="F1793" s="6">
+        <v>1613.8275235863998</v>
+      </c>
+      <c r="H1793" s="6">
+        <v>3.6882067021992984</v>
+      </c>
+      <c r="J1793" s="6">
+        <v>26.98285495429311</v>
+      </c>
+      <c r="K1793" s="6">
+        <v>6.7655143755072844</v>
+      </c>
+      <c r="L1793" s="6">
+        <v>2.8254771647714318</v>
+      </c>
+      <c r="M1793" s="6">
+        <v>16.873919297464262</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1794" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1794" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1794" s="6">
+        <v>2393.4001454042077</v>
+      </c>
+      <c r="D1794" s="6">
+        <v>97.147338929838767</v>
+      </c>
+      <c r="E1794" s="6">
+        <v>68.249304809132909</v>
+      </c>
+      <c r="F1794" s="6">
+        <v>2092.6113018408805</v>
+      </c>
+      <c r="H1794" s="6">
+        <v>1.4298209665319634</v>
+      </c>
+      <c r="J1794" s="6">
+        <v>30.358280042850168</v>
+      </c>
+      <c r="K1794" s="6">
+        <v>3.9778610757267869</v>
+      </c>
+      <c r="L1794" s="6">
+        <v>1.5495087981565627</v>
+      </c>
+      <c r="M1794" s="6">
+        <v>22.503874284755263</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1795" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1795" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1795" s="6">
+        <v>1398.5841159482557</v>
+      </c>
+      <c r="D1795" s="6">
+        <v>214.32903681120865</v>
+      </c>
+      <c r="E1795" s="6">
+        <v>220.95789360669681</v>
+      </c>
+      <c r="F1795" s="6">
+        <v>907.15392268198536</v>
+      </c>
+      <c r="H1795" s="6">
+        <v>3.316276300272698</v>
+      </c>
+      <c r="J1795" s="6">
+        <v>20.040352933903886</v>
+      </c>
+      <c r="K1795" s="6">
+        <v>6.3010432439214812</v>
+      </c>
+      <c r="L1795" s="6">
+        <v>2.1776424209832941</v>
+      </c>
+      <c r="M1795" s="6">
+        <v>11.001030315116997</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1796" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1796" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1796" s="6">
+        <v>2003.555595145102</v>
+      </c>
+      <c r="D1796" s="6">
+        <v>175.64266272709727</v>
+      </c>
+      <c r="E1796" s="6">
+        <v>200.23304567601215</v>
+      </c>
+      <c r="F1796" s="6">
+        <v>1586.2662209943876</v>
+      </c>
+      <c r="H1796" s="6">
+        <v>3.519519668174373</v>
+      </c>
+      <c r="J1796" s="6">
+        <v>25.531009253321109</v>
+      </c>
+      <c r="K1796" s="6">
+        <v>6.2369447033602921</v>
+      </c>
+      <c r="L1796" s="6">
+        <v>2.4329946661117727</v>
+      </c>
+      <c r="M1796" s="6">
+        <v>16.459038708440957</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1797" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1797" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1797" s="6">
+        <v>2595.4989012665833</v>
+      </c>
+      <c r="D1797" s="6">
+        <v>124.30299481797699</v>
+      </c>
+      <c r="E1797" s="6">
+        <v>89.754245961462715</v>
+      </c>
+      <c r="F1797" s="6">
+        <v>2164.7586714060863</v>
+      </c>
+      <c r="H1797" s="6">
+        <v>1.7382793709840021</v>
+      </c>
+      <c r="J1797" s="6">
+        <v>36.648789873689161</v>
+      </c>
+      <c r="K1797" s="6">
+        <v>5.0766860951849289</v>
+      </c>
+      <c r="L1797" s="6">
+        <v>2.1805325695340612</v>
+      </c>
+      <c r="M1797" s="6">
+        <v>26.090945210870508</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1798" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1798" s="5">
+        <v>42752</v>
+      </c>
+      <c r="C1798" s="6">
+        <v>1301.9483472514264</v>
+      </c>
+      <c r="D1798" s="6">
+        <v>221.18053444787424</v>
+      </c>
+      <c r="E1798" s="6">
+        <v>236.3937373196965</v>
+      </c>
+      <c r="F1798" s="6">
+        <v>798.55991755747846</v>
+      </c>
+      <c r="H1798" s="6">
+        <v>3.4831527165851797</v>
+      </c>
+      <c r="J1798" s="6">
+        <v>20.005453193471418</v>
+      </c>
+      <c r="K1798" s="6">
+        <v>6.3039394662566588</v>
+      </c>
+      <c r="L1798" s="6">
+        <v>2.6257443208398827</v>
+      </c>
+      <c r="M1798" s="6">
+        <v>10.506824553206677</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1799" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1799" s="5">
+        <v>42786</v>
+      </c>
+      <c r="C1799" s="6">
+        <v>2073.6811469834965</v>
+      </c>
+      <c r="D1799" s="6">
+        <v>256.55493692109809</v>
+      </c>
+      <c r="E1799" s="6">
+        <v>292.32558202714779</v>
+      </c>
+      <c r="F1799" s="6">
+        <v>1459.1785999162944</v>
+      </c>
+      <c r="H1799" s="6">
+        <v>4.6608820139436835</v>
+      </c>
+      <c r="J1799" s="6">
+        <v>33.049359398382919</v>
+      </c>
+      <c r="K1799" s="6">
+        <v>9.4926359837896417</v>
+      </c>
+      <c r="L1799" s="6">
+        <v>4.0061838379744357</v>
+      </c>
+      <c r="M1799" s="6">
+        <v>18.885281631225958</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1800" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1800" s="5">
+        <v>42884</v>
+      </c>
+      <c r="C1800" s="6">
+        <v>2398.7818164776299</v>
+      </c>
+      <c r="D1800" s="6">
+        <v>124.27741753471389</v>
+      </c>
+      <c r="E1800" s="6">
+        <v>91.403144530707777</v>
+      </c>
+      <c r="F1800" s="6">
+        <v>2002.1876545517382</v>
+      </c>
+      <c r="H1800" s="6">
+        <v>1.6390139988115209</v>
+      </c>
+      <c r="J1800" s="6">
+        <v>40.013030184706366</v>
+      </c>
+      <c r="K1800" s="6">
+        <v>4.9596428920268041</v>
+      </c>
+      <c r="L1800" s="6">
+        <v>2.2306633695973761</v>
+      </c>
+      <c r="M1800" s="6">
+        <v>29.34747969149414</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1801" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1801" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1801" s="6">
+        <v>11.847026662531761</v>
+      </c>
+      <c r="D1801" s="6">
+        <v>7.6757637352438852</v>
+      </c>
+      <c r="E1801" s="6">
+        <v>2.5848938326155992</v>
+      </c>
+      <c r="F1801" s="6">
+        <v>1.5863690946722762</v>
+      </c>
+      <c r="H1801" s="6">
+        <v>0.10272981229717383</v>
+      </c>
+      <c r="J1801" s="6">
+        <v>0.49774354496410211</v>
+      </c>
+      <c r="K1801" s="6">
+        <v>0.33789188904612055</v>
+      </c>
+      <c r="L1801" s="6">
+        <v>0.11334352957270555</v>
+      </c>
+      <c r="M1801" s="6">
+        <v>4.6508126345276041E-2</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1802" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1802" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1802" s="6">
+        <v>249.24832591592448</v>
+      </c>
+      <c r="D1802" s="6">
+        <v>105.44962100551689</v>
+      </c>
+      <c r="E1802" s="6">
+        <v>50.258450417885577</v>
+      </c>
+      <c r="F1802" s="6">
+        <v>89.493768278915681</v>
+      </c>
+      <c r="H1802" s="6">
+        <v>1.632680477012076</v>
+      </c>
+      <c r="J1802" s="6">
+        <v>7.7745085272611947</v>
+      </c>
+      <c r="K1802" s="6">
+        <v>4.3865201154210833</v>
+      </c>
+      <c r="L1802" s="6">
+        <v>1.5921583062052593</v>
+      </c>
+      <c r="M1802" s="6">
+        <v>1.7388543749385348</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1803" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1803" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1803" s="6">
+        <v>1460.8973022296786</v>
+      </c>
+      <c r="D1803" s="6">
+        <v>184.92482371305584</v>
+      </c>
+      <c r="E1803" s="6">
+        <v>203.03456441138513</v>
+      </c>
+      <c r="F1803" s="6">
+        <v>1043.5187556511571</v>
+      </c>
+      <c r="H1803" s="6">
+        <v>2.967891404258225</v>
+      </c>
+      <c r="J1803" s="6">
+        <v>24.557079450678199</v>
+      </c>
+      <c r="K1803" s="6">
+        <v>7.3284295008966778</v>
+      </c>
+      <c r="L1803" s="6">
+        <v>4.0161788573879447</v>
+      </c>
+      <c r="M1803" s="6">
+        <v>12.76832158506668</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1804" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1804" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1804" s="6">
+        <v>17.529053397009744</v>
+      </c>
+      <c r="D1804" s="6">
+        <v>11.353270560726354</v>
+      </c>
+      <c r="E1804" s="6">
+        <v>3.5644308668156874</v>
+      </c>
+      <c r="F1804" s="6">
+        <v>2.6113519694677034</v>
+      </c>
+      <c r="H1804" s="6">
+        <v>0.16219347101491013</v>
+      </c>
+      <c r="J1804" s="6">
+        <v>0.74497125168862222</v>
+      </c>
+      <c r="K1804" s="6">
+        <v>0.50793643929296739</v>
+      </c>
+      <c r="L1804" s="6">
+        <v>0.16088399488891578</v>
+      </c>
+      <c r="M1804" s="6">
+        <v>7.6150817506739146E-2</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1805" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1805" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1805" s="6">
+        <v>308.69262133750772</v>
+      </c>
+      <c r="D1805" s="6">
+        <v>115.6218433624955</v>
+      </c>
+      <c r="E1805" s="6">
+        <v>83.296721130333523</v>
+      </c>
+      <c r="F1805" s="6">
+        <v>106.31636707020819</v>
+      </c>
+      <c r="H1805" s="6">
+        <v>2.0002079690206602</v>
+      </c>
+      <c r="J1805" s="6">
+        <v>10.232137880473658</v>
+      </c>
+      <c r="K1805" s="6">
+        <v>5.1007121623827176</v>
+      </c>
+      <c r="L1805" s="6">
+        <v>2.889868567851269</v>
+      </c>
+      <c r="M1805" s="6">
+        <v>2.1916458191996706</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1806" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1806" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1806" s="6">
+        <v>1657.8086736523887</v>
+      </c>
+      <c r="D1806" s="6">
+        <v>283.22823640489167</v>
+      </c>
+      <c r="E1806" s="6">
+        <v>303.94705475894773</v>
+      </c>
+      <c r="F1806" s="6">
+        <v>1059.2275589725496</v>
+      </c>
+      <c r="H1806" s="6">
+        <v>4.2993779135734789</v>
+      </c>
+      <c r="J1806" s="6">
+        <v>32.997377452828161</v>
+      </c>
+      <c r="K1806" s="6">
+        <v>11.157375570190583</v>
+      </c>
+      <c r="L1806" s="6">
+        <v>7.0411839605146991</v>
+      </c>
+      <c r="M1806" s="6">
+        <v>14.625541883301295</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1807" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1807" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1807" s="6">
+        <v>10.952226954935341</v>
+      </c>
+      <c r="D1807" s="6">
+        <v>7.0440799544166355</v>
+      </c>
+      <c r="E1807" s="6">
+        <v>2.4363223207327009</v>
+      </c>
+      <c r="F1807" s="6">
+        <v>1.4718246797860037</v>
+      </c>
+      <c r="H1807" s="6">
+        <v>9.7615472463160977E-2</v>
+      </c>
+      <c r="J1807" s="6">
+        <v>0.45949446731893967</v>
+      </c>
+      <c r="K1807" s="6">
+        <v>0.30741727047801554</v>
+      </c>
+      <c r="L1807" s="6">
+        <v>0.10724173770212664</v>
+      </c>
+      <c r="M1807" s="6">
+        <v>4.4835459138797371E-2</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1808" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1808" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1808" s="6">
+        <v>232.14684858619461</v>
+      </c>
+      <c r="D1808" s="6">
+        <v>89.088180699312488</v>
+      </c>
+      <c r="E1808" s="6">
+        <v>52.059647846722953</v>
+      </c>
+      <c r="F1808" s="6">
+        <v>88.450697850401951</v>
+      </c>
+      <c r="H1808" s="6">
+        <v>1.5150369537240171</v>
+      </c>
+      <c r="J1808" s="6">
+        <v>7.9890866806582821</v>
+      </c>
+      <c r="K1808" s="6">
+        <v>4.1386933915987791</v>
+      </c>
+      <c r="L1808" s="6">
+        <v>1.9170590684234099</v>
+      </c>
+      <c r="M1808" s="6">
+        <v>1.8850568093819624</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1809" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1809" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1809" s="6">
+        <v>1489.1916962056384</v>
+      </c>
+      <c r="D1809" s="6">
+        <v>237.06158342334942</v>
+      </c>
+      <c r="E1809" s="6">
+        <v>276.39004500070189</v>
+      </c>
+      <c r="F1809" s="6">
+        <v>943.78818898990232</v>
+      </c>
+      <c r="H1809" s="6">
+        <v>4.0741744631555283</v>
+      </c>
+      <c r="J1809" s="6">
+        <v>32.024879637835603</v>
+      </c>
+      <c r="K1809" s="6">
+        <v>10.184748854400398</v>
+      </c>
+      <c r="L1809" s="6">
+        <v>6.9026863601907831</v>
+      </c>
+      <c r="M1809" s="6">
+        <v>14.271252497827899</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1810" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1810" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1810" s="6">
+        <v>16.348483927217995</v>
+      </c>
+      <c r="D1810" s="6">
+        <v>10.852751623932305</v>
+      </c>
+      <c r="E1810" s="6">
+        <v>3.2998352014616699</v>
+      </c>
+      <c r="F1810" s="6">
+        <v>2.195897101824019</v>
+      </c>
+      <c r="H1810" s="6">
+        <v>0.14751376276722425</v>
+      </c>
+      <c r="J1810" s="6">
+        <v>0.70726819541436159</v>
+      </c>
+      <c r="K1810" s="6">
+        <v>0.49258111632820978</v>
+      </c>
+      <c r="L1810" s="6">
+        <v>0.15129485393437089</v>
+      </c>
+      <c r="M1810" s="6">
+        <v>6.3392225151780987E-2</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1811" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1811" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1811" s="6">
+        <v>263.33741315948322</v>
+      </c>
+      <c r="D1811" s="6">
+        <v>102.46684419664061</v>
+      </c>
+      <c r="E1811" s="6">
+        <v>53.499563831096658</v>
+      </c>
+      <c r="F1811" s="6">
+        <v>104.58020611957143</v>
+      </c>
+      <c r="H1811" s="6">
+        <v>1.5715461985951469</v>
+      </c>
+      <c r="J1811" s="6">
+        <v>8.6609650430703446</v>
+      </c>
+      <c r="K1811" s="6">
+        <v>4.5337002824463619</v>
+      </c>
+      <c r="L1811" s="6">
+        <v>1.9259948967735798</v>
+      </c>
+      <c r="M1811" s="6">
+        <v>2.1546928492257118</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1812" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1812" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1812" s="6">
+        <v>1483.1963470335209</v>
+      </c>
+      <c r="D1812" s="6">
+        <v>277.5208286182214</v>
+      </c>
+      <c r="E1812" s="6">
+        <v>218.49056127783351</v>
+      </c>
+      <c r="F1812" s="6">
+        <v>973.65926132323511</v>
+      </c>
+      <c r="H1812" s="6">
+        <v>4.5008061038632663</v>
+      </c>
+      <c r="J1812" s="6">
+        <v>33.400321374068476</v>
+      </c>
+      <c r="K1812" s="6">
+        <v>12.658423083535862</v>
+      </c>
+      <c r="L1812" s="6">
+        <v>5.7076245361241869</v>
+      </c>
+      <c r="M1812" s="6">
+        <v>14.734499753143462</v>
+      </c>
+    </row>
+    <row r="1813" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1813" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1813" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1813" s="6">
+        <v>11.847026662531761</v>
+      </c>
+      <c r="D1813" s="6">
+        <v>7.6757637352438852</v>
+      </c>
+      <c r="E1813" s="6">
+        <v>2.5848938326155992</v>
+      </c>
+      <c r="F1813" s="6">
+        <v>1.5863690946722762</v>
+      </c>
+      <c r="H1813" s="6">
+        <v>0.10272981229717383</v>
+      </c>
+      <c r="J1813" s="6">
+        <v>0.49774354496410211</v>
+      </c>
+      <c r="K1813" s="6">
+        <v>0.33789188904612055</v>
+      </c>
+      <c r="L1813" s="6">
+        <v>0.11334352957270555</v>
+      </c>
+      <c r="M1813" s="6">
+        <v>4.6508126345276041E-2</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1814" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1814" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1814" s="6">
+        <v>249.24832591592448</v>
+      </c>
+      <c r="D1814" s="6">
+        <v>105.44962100551689</v>
+      </c>
+      <c r="E1814" s="6">
+        <v>50.258450417885577</v>
+      </c>
+      <c r="F1814" s="6">
+        <v>89.493768278915681</v>
+      </c>
+      <c r="H1814" s="6">
+        <v>1.632680477012076</v>
+      </c>
+      <c r="J1814" s="6">
+        <v>7.7745085272611947</v>
+      </c>
+      <c r="K1814" s="6">
+        <v>4.3865201154210833</v>
+      </c>
+      <c r="L1814" s="6">
+        <v>1.5921583062052593</v>
+      </c>
+      <c r="M1814" s="6">
+        <v>1.7388543749385348</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1815" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1815" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1815" s="6">
+        <v>1460.8973022296786</v>
+      </c>
+      <c r="D1815" s="6">
+        <v>184.92482371305584</v>
+      </c>
+      <c r="E1815" s="6">
+        <v>203.03456441138513</v>
+      </c>
+      <c r="F1815" s="6">
+        <v>1043.5187556511571</v>
+      </c>
+      <c r="H1815" s="6">
+        <v>2.967891404258225</v>
+      </c>
+      <c r="J1815" s="6">
+        <v>24.557079450678199</v>
+      </c>
+      <c r="K1815" s="6">
+        <v>7.3284295008966778</v>
+      </c>
+      <c r="L1815" s="6">
+        <v>4.0161788573879447</v>
+      </c>
+      <c r="M1815" s="6">
+        <v>12.76832158506668</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1816" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1816" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1816" s="6">
+        <v>10.665873262676099</v>
+      </c>
+      <c r="D1816" s="6">
+        <v>7.0092549446841259</v>
+      </c>
+      <c r="E1816" s="6">
+        <v>2.2356136812264329</v>
+      </c>
+      <c r="F1816" s="6">
+        <v>1.4210046367655416</v>
+      </c>
+      <c r="H1816" s="6">
+        <v>9.4620704526704888E-2</v>
+      </c>
+      <c r="J1816" s="6">
+        <v>0.4519159877944845</v>
+      </c>
+      <c r="K1816" s="6">
+        <v>0.30773499791585923</v>
+      </c>
+      <c r="L1816" s="6">
+        <v>9.8997257723958884E-2</v>
+      </c>
+      <c r="M1816" s="6">
+        <v>4.518373215466643E-2</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1817" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1817" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1817" s="6">
+        <v>234.56698061406246</v>
+      </c>
+      <c r="D1817" s="6">
+        <v>102.39235036911387</v>
+      </c>
+      <c r="E1817" s="6">
+        <v>49.908103156831764</v>
+      </c>
+      <c r="F1817" s="6">
+        <v>79.767861864593172</v>
+      </c>
+      <c r="H1817" s="6">
+        <v>1.5657448849784867</v>
+      </c>
+      <c r="J1817" s="6">
+        <v>7.8155367548115411</v>
+      </c>
+      <c r="K1817" s="6">
+        <v>4.4386280143662695</v>
+      </c>
+      <c r="L1817" s="6">
+        <v>1.7328724837914364</v>
+      </c>
+      <c r="M1817" s="6">
+        <v>1.6119658464486566</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1818" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1818" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1818" s="6">
+        <v>1262.6153278481743</v>
+      </c>
+      <c r="D1818" s="6">
+        <v>209.22197133117683</v>
+      </c>
+      <c r="E1818" s="6">
+        <v>223.2963413964429</v>
+      </c>
+      <c r="F1818" s="6">
+        <v>814.5712832524548</v>
+      </c>
+      <c r="H1818" s="6">
+        <v>3.6863423497165928</v>
+      </c>
+      <c r="J1818" s="6">
+        <v>24.167589525954899</v>
+      </c>
+      <c r="K1818" s="6">
+        <v>8.2443350559095947</v>
+      </c>
+      <c r="L1818" s="6">
+        <v>4.7994461331347678</v>
+      </c>
+      <c r="M1818" s="6">
+        <v>10.863037517205044</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1819" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1819" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1819" s="6">
+        <v>7.9964209534157007</v>
+      </c>
+      <c r="D1819" s="6">
+        <v>5.1785383653716002</v>
+      </c>
+      <c r="E1819" s="6">
+        <v>1.8238051781888012</v>
+      </c>
+      <c r="F1819" s="6">
+        <v>0.99407740985529824</v>
+      </c>
+      <c r="H1819" s="6">
+        <v>7.5038422489478659E-2</v>
+      </c>
+      <c r="J1819" s="6">
+        <v>0.34909283284891929</v>
+      </c>
+      <c r="K1819" s="6">
+        <v>0.23359235057227851</v>
+      </c>
+      <c r="L1819" s="6">
+        <v>8.3961445487928138E-2</v>
+      </c>
+      <c r="M1819" s="6">
+        <v>3.1539036788712664E-2</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1820" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1820" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1820" s="6">
+        <v>271.68024657368613</v>
+      </c>
+      <c r="D1820" s="6">
+        <v>98.049828826803804</v>
+      </c>
+      <c r="E1820" s="6">
+        <v>49.853712718419729</v>
+      </c>
+      <c r="F1820" s="6">
+        <v>120.53033452856096</v>
+      </c>
+      <c r="H1820" s="6">
+        <v>1.5390868331415459</v>
+      </c>
+      <c r="J1820" s="6">
+        <v>8.7767397174049826</v>
+      </c>
+      <c r="K1820" s="6">
+        <v>4.4993018555942879</v>
+      </c>
+      <c r="L1820" s="6">
+        <v>1.7957967821156728</v>
+      </c>
+      <c r="M1820" s="6">
+        <v>2.432552648971559</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1821" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1821" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1821" s="6">
+        <v>1446.1451328099899</v>
+      </c>
+      <c r="D1821" s="6">
+        <v>275.16122788775317</v>
+      </c>
+      <c r="E1821" s="6">
+        <v>232.57957811265328</v>
+      </c>
+      <c r="F1821" s="6">
+        <v>930.96693855493891</v>
+      </c>
+      <c r="H1821" s="6">
+        <v>4.22697063923495</v>
+      </c>
+      <c r="J1821" s="6">
+        <v>32.079992217921202</v>
+      </c>
+      <c r="K1821" s="6">
+        <v>11.802396964378062</v>
+      </c>
+      <c r="L1821" s="6">
+        <v>5.8603773512309001</v>
+      </c>
+      <c r="M1821" s="6">
+        <v>14.236460516969833</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1822" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1822" s="5">
+        <v>42759</v>
+      </c>
+      <c r="C1822" s="6">
+        <v>10.042536323922798</v>
+      </c>
+      <c r="D1822" s="6">
+        <v>6.4080925752783475</v>
+      </c>
+      <c r="E1822" s="6">
+        <v>2.3958144299500264</v>
+      </c>
+      <c r="F1822" s="6">
+        <v>1.2386293186944264</v>
+      </c>
+      <c r="H1822" s="6">
+        <v>9.3600044050185641E-2</v>
+      </c>
+      <c r="J1822" s="6">
+        <v>0.42361800981614506</v>
+      </c>
+      <c r="K1822" s="6">
+        <v>0.28435829995440715</v>
+      </c>
+      <c r="L1822" s="6">
+        <v>0.1022557975622238</v>
+      </c>
+      <c r="M1822" s="6">
+        <v>3.7003912299514094E-2</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1823" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1823" s="5">
+        <v>42794</v>
+      </c>
+      <c r="C1823" s="6">
+        <v>250.77943417107193</v>
+      </c>
+      <c r="D1823" s="6">
+        <v>102.18057155442983</v>
+      </c>
+      <c r="E1823" s="6">
+        <v>52.936694272514238</v>
+      </c>
+      <c r="F1823" s="6">
+        <v>92.459037080963611</v>
+      </c>
+      <c r="H1823" s="6">
+        <v>1.6314164156127138</v>
+      </c>
+      <c r="J1823" s="6">
+        <v>8.5364757359032311</v>
+      </c>
+      <c r="K1823" s="6">
+        <v>4.6623471228415294</v>
+      </c>
+      <c r="L1823" s="6">
+        <v>1.9085710892430445</v>
+      </c>
+      <c r="M1823" s="6">
+        <v>1.9217910634916637</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1824" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1824" s="5">
+        <v>42864</v>
+      </c>
+      <c r="C1824" s="6">
+        <v>1411.860684613182</v>
+      </c>
+      <c r="D1824" s="6">
+        <v>243.73576380223753</v>
+      </c>
+      <c r="E1824" s="6">
+        <v>189.99018975419966</v>
+      </c>
+      <c r="F1824" s="6">
+        <v>961.69914908347505</v>
+      </c>
+      <c r="H1824" s="6">
+        <v>3.4770875240793395</v>
+      </c>
+      <c r="J1824" s="6">
+        <v>33.245322695714314</v>
+      </c>
+      <c r="K1824" s="6">
+        <v>10.865148175979114</v>
+      </c>
+      <c r="L1824" s="6">
+        <v>5.3270712621327601</v>
+      </c>
+      <c r="M1824" s="6">
+        <v>16.635788172135083</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1825" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1825" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1825" s="6">
+        <v>743.03604645554924</v>
+      </c>
+      <c r="D1825" s="6">
+        <v>217.03991539652083</v>
+      </c>
+      <c r="E1825" s="6">
+        <v>120.99425212732793</v>
+      </c>
+      <c r="F1825" s="6">
+        <v>382.85695552079875</v>
+      </c>
+      <c r="H1825" s="6">
+        <v>2.9421700660880639</v>
+      </c>
+      <c r="J1825" s="6">
+        <v>20.172906973896211</v>
+      </c>
+      <c r="K1825" s="6">
+        <v>8.872093693386006</v>
+      </c>
+      <c r="L1825" s="6">
+        <v>3.4432935985234585</v>
+      </c>
+      <c r="M1825" s="6">
+        <v>7.5320410184990774</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1826" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1826" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1826" s="6">
+        <v>1432.3921214872132</v>
+      </c>
+      <c r="D1826" s="6">
+        <v>174.31647238356476</v>
+      </c>
+      <c r="E1826" s="6">
+        <v>200.37302569923412</v>
+      </c>
+      <c r="F1826" s="6">
+        <v>1017.2151720675158</v>
+      </c>
+      <c r="H1826" s="6">
+        <v>3.0211375711355508</v>
+      </c>
+      <c r="J1826" s="6">
+        <v>21.507650153897188</v>
+      </c>
+      <c r="K1826" s="6">
+        <v>6.2882796121419204</v>
+      </c>
+      <c r="L1826" s="6">
+        <v>2.8990441539295797</v>
+      </c>
+      <c r="M1826" s="6">
+        <v>11.922886226005799</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1827" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1827" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1827" s="6">
+        <v>1904.0715937285781</v>
+      </c>
+      <c r="D1827" s="6">
+        <v>154.12821889279601</v>
+      </c>
+      <c r="E1827" s="6">
+        <v>151.14157847933669</v>
+      </c>
+      <c r="F1827" s="6">
+        <v>1515.5262394012555</v>
+      </c>
+      <c r="H1827" s="6">
+        <v>3.0275299374791644</v>
+      </c>
+      <c r="J1827" s="6">
+        <v>26.819171735766027</v>
+      </c>
+      <c r="K1827" s="6">
+        <v>6.0415143995193095</v>
+      </c>
+      <c r="L1827" s="6">
+        <v>2.7651849414298981</v>
+      </c>
+      <c r="M1827" s="6">
+        <v>16.936934678447276</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1828" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1828" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1828" s="6">
+        <v>765.63176148977755</v>
+      </c>
+      <c r="D1828" s="6">
+        <v>232.70049792682454</v>
+      </c>
+      <c r="E1828" s="6">
+        <v>131.76611633567839</v>
+      </c>
+      <c r="F1828" s="6">
+        <v>387.84233348748199</v>
+      </c>
+      <c r="H1828" s="6">
+        <v>3.3195614252860537</v>
+      </c>
+      <c r="J1828" s="6">
+        <v>21.580910419800908</v>
+      </c>
+      <c r="K1828" s="6">
+        <v>9.8475036204821844</v>
+      </c>
+      <c r="L1828" s="6">
+        <v>3.7513056170477661</v>
+      </c>
+      <c r="M1828" s="6">
+        <v>7.7889278081540834</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1829" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1829" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1829" s="6">
+        <v>1398.49015068832</v>
+      </c>
+      <c r="D1829" s="6">
+        <v>156.95378060936503</v>
+      </c>
+      <c r="E1829" s="6">
+        <v>165.61725457709036</v>
+      </c>
+      <c r="F1829" s="6">
+        <v>1043.1214267782254</v>
+      </c>
+      <c r="H1829" s="6">
+        <v>2.9068205904878206</v>
+      </c>
+      <c r="J1829" s="6">
+        <v>22.503799933172377</v>
+      </c>
+      <c r="K1829" s="6">
+        <v>5.5990735914027114</v>
+      </c>
+      <c r="L1829" s="6">
+        <v>2.4615595245234165</v>
+      </c>
+      <c r="M1829" s="6">
+        <v>14.138480828251724</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1830" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1830" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1830" s="6">
+        <v>1950.8549435669177</v>
+      </c>
+      <c r="D1830" s="6">
+        <v>155.63261128039628</v>
+      </c>
+      <c r="E1830" s="6">
+        <v>153.97885691071696</v>
+      </c>
+      <c r="F1830" s="6">
+        <v>1571.3044793336032</v>
+      </c>
+      <c r="H1830" s="6">
+        <v>2.8489073373592526</v>
+      </c>
+      <c r="J1830" s="6">
+        <v>28.315091276405116</v>
+      </c>
+      <c r="K1830" s="6">
+        <v>5.7995637670638986</v>
+      </c>
+      <c r="L1830" s="6">
+        <v>3.1317772598681715</v>
+      </c>
+      <c r="M1830" s="6">
+        <v>18.53311616027479</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1831" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1831" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1831" s="6">
+        <v>539.24373384873343</v>
+      </c>
+      <c r="D1831" s="6">
+        <v>176.17649544305252</v>
+      </c>
+      <c r="E1831" s="6">
+        <v>95.272675258031171</v>
+      </c>
+      <c r="F1831" s="6">
+        <v>255.56225974694226</v>
+      </c>
+      <c r="H1831" s="6">
+        <v>2.6716401276666857</v>
+      </c>
+      <c r="J1831" s="6">
+        <v>16.027178037274528</v>
+      </c>
+      <c r="K1831" s="6">
+        <v>7.6998950652659648</v>
+      </c>
+      <c r="L1831" s="6">
+        <v>2.9384697418413945</v>
+      </c>
+      <c r="M1831" s="6">
+        <v>5.2284423306967565</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1832" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1832" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1832" s="6">
+        <v>1457.7222771830598</v>
+      </c>
+      <c r="D1832" s="6">
+        <v>150.24718511347709</v>
+      </c>
+      <c r="E1832" s="6">
+        <v>172.40115366328203</v>
+      </c>
+      <c r="F1832" s="6">
+        <v>1087.4425328950356</v>
+      </c>
+      <c r="H1832" s="6">
+        <v>2.7480651798640729</v>
+      </c>
+      <c r="J1832" s="6">
+        <v>27.206648090510907</v>
+      </c>
+      <c r="K1832" s="6">
+        <v>6.3899211433843837</v>
+      </c>
+      <c r="L1832" s="6">
+        <v>3.2262971452424929</v>
+      </c>
+      <c r="M1832" s="6">
+        <v>16.992993346324397</v>
+      </c>
+    </row>
+    <row r="1833" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1833" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1833" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1833" s="6">
+        <v>2137.2914952511464</v>
+      </c>
+      <c r="D1833" s="6">
+        <v>192.44889492250377</v>
+      </c>
+      <c r="E1833" s="6">
+        <v>208.40938983051586</v>
+      </c>
+      <c r="F1833" s="6">
+        <v>1665.4060184012119</v>
+      </c>
+      <c r="H1833" s="6">
+        <v>3.5802237876238556</v>
+      </c>
+      <c r="J1833" s="6">
+        <v>33.113968162533524</v>
+      </c>
+      <c r="K1833" s="6">
+        <v>7.5844782759342859</v>
+      </c>
+      <c r="L1833" s="6">
+        <v>4.0374052597384171</v>
+      </c>
+      <c r="M1833" s="6">
+        <v>20.521933852169749</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1834" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1834" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1834" s="6">
+        <v>765.94581967745762</v>
+      </c>
+      <c r="D1834" s="6">
+        <v>241.93756911042769</v>
+      </c>
+      <c r="E1834" s="6">
+        <v>140.85971722192397</v>
+      </c>
+      <c r="F1834" s="6">
+        <v>359.77094779971242</v>
+      </c>
+      <c r="H1834" s="6">
+        <v>3.4680548742858863</v>
+      </c>
+      <c r="J1834" s="6">
+        <v>21.242485692861088</v>
+      </c>
+      <c r="K1834" s="6">
+        <v>9.587212936560114</v>
+      </c>
+      <c r="L1834" s="6">
+        <v>4.1100942626770074</v>
+      </c>
+      <c r="M1834" s="6">
+        <v>7.1852780663097846</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1835" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1835" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1835" s="6">
+        <v>1430.6866691078042</v>
+      </c>
+      <c r="D1835" s="6">
+        <v>174.16407907662852</v>
+      </c>
+      <c r="E1835" s="6">
+        <v>212.82726761783994</v>
+      </c>
+      <c r="F1835" s="6">
+        <v>996.96113450214068</v>
+      </c>
+      <c r="H1835" s="6">
+        <v>3.0959021114851986</v>
+      </c>
+      <c r="J1835" s="6">
+        <v>25.332491855319873</v>
+      </c>
+      <c r="K1835" s="6">
+        <v>6.7997698342227277</v>
+      </c>
+      <c r="L1835" s="6">
+        <v>3.4509303991555269</v>
+      </c>
+      <c r="M1835" s="6">
+        <v>14.490532442544062</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1836" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1836" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1836" s="6">
+        <v>2128.1296336220494</v>
+      </c>
+      <c r="D1836" s="6">
+        <v>202.09964770990842</v>
+      </c>
+      <c r="E1836" s="6">
+        <v>219.74198798871052</v>
+      </c>
+      <c r="F1836" s="6">
+        <v>1631.1167301061062</v>
+      </c>
+      <c r="H1836" s="6">
+        <v>3.547481693330957</v>
+      </c>
+      <c r="J1836" s="6">
+        <v>31.712305350193862</v>
+      </c>
+      <c r="K1836" s="6">
+        <v>7.2478262266064233</v>
+      </c>
+      <c r="L1836" s="6">
+        <v>3.5639924107872694</v>
+      </c>
+      <c r="M1836" s="6">
+        <v>20.000298849931536</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1837" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1837" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1837" s="6">
+        <v>743.03604645554924</v>
+      </c>
+      <c r="D1837" s="6">
+        <v>217.03991539652083</v>
+      </c>
+      <c r="E1837" s="6">
+        <v>120.99425212732793</v>
+      </c>
+      <c r="F1837" s="6">
+        <v>382.85695552079875</v>
+      </c>
+      <c r="H1837" s="6">
+        <v>2.9421700660880639</v>
+      </c>
+      <c r="J1837" s="6">
+        <v>20.172906973896211</v>
+      </c>
+      <c r="K1837" s="6">
+        <v>8.872093693386006</v>
+      </c>
+      <c r="L1837" s="6">
+        <v>3.4432935985234585</v>
+      </c>
+      <c r="M1837" s="6">
+        <v>7.5320410184990774</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1838" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1838" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1838" s="6">
+        <v>1432.3921214872132</v>
+      </c>
+      <c r="D1838" s="6">
+        <v>174.31647238356476</v>
+      </c>
+      <c r="E1838" s="6">
+        <v>200.37302569923412</v>
+      </c>
+      <c r="F1838" s="6">
+        <v>1017.2151720675158</v>
+      </c>
+      <c r="H1838" s="6">
+        <v>3.0211375711355508</v>
+      </c>
+      <c r="J1838" s="6">
+        <v>21.507650153897188</v>
+      </c>
+      <c r="K1838" s="6">
+        <v>6.2882796121419204</v>
+      </c>
+      <c r="L1838" s="6">
+        <v>2.8990441539295797</v>
+      </c>
+      <c r="M1838" s="6">
+        <v>11.922886226005799</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1839" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1839" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1839" s="6">
+        <v>1904.0715937285781</v>
+      </c>
+      <c r="D1839" s="6">
+        <v>154.12821889279601</v>
+      </c>
+      <c r="E1839" s="6">
+        <v>151.14157847933669</v>
+      </c>
+      <c r="F1839" s="6">
+        <v>1515.5262394012555</v>
+      </c>
+      <c r="H1839" s="6">
+        <v>3.0275299374791644</v>
+      </c>
+      <c r="J1839" s="6">
+        <v>26.819171735766027</v>
+      </c>
+      <c r="K1839" s="6">
+        <v>6.0415143995193095</v>
+      </c>
+      <c r="L1839" s="6">
+        <v>2.7651849414298981</v>
+      </c>
+      <c r="M1839" s="6">
+        <v>16.936934678447276</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1840" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1840" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1840" s="6">
+        <v>810.32960154714874</v>
+      </c>
+      <c r="D1840" s="6">
+        <v>257.74955944643227</v>
+      </c>
+      <c r="E1840" s="6">
+        <v>152.0936267345009</v>
+      </c>
+      <c r="F1840" s="6">
+        <v>385.93364123935078</v>
+      </c>
+      <c r="H1840" s="6">
+        <v>3.5235473784390661</v>
+      </c>
+      <c r="J1840" s="6">
+        <v>22.450876430717958</v>
+      </c>
+      <c r="K1840" s="6">
+        <v>10.62808711892799</v>
+      </c>
+      <c r="L1840" s="6">
+        <v>4.1244631334516688</v>
+      </c>
+      <c r="M1840" s="6">
+        <v>7.4791008931645262</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1841" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1841" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1841" s="6">
+        <v>1272.0522168081147</v>
+      </c>
+      <c r="D1841" s="6">
+        <v>137.37768956355973</v>
+      </c>
+      <c r="E1841" s="6">
+        <v>142.64686061457951</v>
+      </c>
+      <c r="F1841" s="6">
+        <v>955.6611810782988</v>
+      </c>
+      <c r="H1841" s="6">
+        <v>2.5044638074299939</v>
+      </c>
+      <c r="J1841" s="6">
+        <v>23.087835824364348</v>
+      </c>
+      <c r="K1841" s="6">
+        <v>5.8000873723344588</v>
+      </c>
+      <c r="L1841" s="6">
+        <v>2.4191698463798788</v>
+      </c>
+      <c r="M1841" s="6">
+        <v>14.428740230861024</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1842" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1842" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1842" s="6">
+        <v>2200.5076043305548</v>
+      </c>
+      <c r="D1842" s="6">
+        <v>205.76432421600197</v>
+      </c>
+      <c r="E1842" s="6">
+        <v>225.78043376468972</v>
+      </c>
+      <c r="F1842" s="6">
+        <v>1678.1727734486817</v>
+      </c>
+      <c r="H1842" s="6">
+        <v>3.6707925868279716</v>
+      </c>
+      <c r="J1842" s="6">
+        <v>36.676454084315907</v>
+      </c>
+      <c r="K1842" s="6">
+        <v>8.214811933357236</v>
+      </c>
+      <c r="L1842" s="6">
+        <v>4.3616841212105175</v>
+      </c>
+      <c r="M1842" s="6">
+        <v>23.01585674691777</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1843" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1843" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1843" s="6">
+        <v>779.46885747457702</v>
+      </c>
+      <c r="D1843" s="6">
+        <v>245.56229618804295</v>
+      </c>
+      <c r="E1843" s="6">
+        <v>124.93239972137958</v>
+      </c>
+      <c r="F1843" s="6">
+        <v>387.39971969340064</v>
+      </c>
+      <c r="H1843" s="6">
+        <v>3.4570281490954251</v>
+      </c>
+      <c r="J1843" s="6">
+        <v>22.882916280304208</v>
+      </c>
+      <c r="K1843" s="6">
+        <v>10.511841847324762</v>
+      </c>
+      <c r="L1843" s="6">
+        <v>3.8866465816951594</v>
+      </c>
+      <c r="M1843" s="6">
+        <v>8.140802263316214</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1844" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1844" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1844" s="6">
+        <v>1408.3451190827568</v>
+      </c>
+      <c r="D1844" s="6">
+        <v>157.70787523520772</v>
+      </c>
+      <c r="E1844" s="6">
+        <v>180.86259671233404</v>
+      </c>
+      <c r="F1844" s="6">
+        <v>1023.2829931818842</v>
+      </c>
+      <c r="H1844" s="6">
+        <v>3.0929060926588083</v>
+      </c>
+      <c r="J1844" s="6">
+        <v>22.927600864411218</v>
+      </c>
+      <c r="K1844" s="6">
+        <v>6.2052977926914838</v>
+      </c>
+      <c r="L1844" s="6">
+        <v>2.8304932982406905</v>
+      </c>
+      <c r="M1844" s="6">
+        <v>13.390053847068074</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1845" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1845" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1845" s="6">
+        <v>1988.2957202663661</v>
+      </c>
+      <c r="D1845" s="6">
+        <v>197.54492901835994</v>
+      </c>
+      <c r="E1845" s="6">
+        <v>183.5121382117666</v>
+      </c>
+      <c r="F1845" s="6">
+        <v>1520.3350448404608</v>
+      </c>
+      <c r="H1845" s="6">
+        <v>3.6663352679753847</v>
+      </c>
+      <c r="J1845" s="6">
+        <v>32.699911122550205</v>
+      </c>
+      <c r="K1845" s="6">
+        <v>7.351886070835981</v>
+      </c>
+      <c r="L1845" s="6">
+        <v>3.6562501626730346</v>
+      </c>
+      <c r="M1845" s="6">
+        <v>20.641925524441795</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1846" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1846" s="5">
+        <v>42748</v>
+      </c>
+      <c r="C1846" s="6">
+        <v>665.16796477769833</v>
+      </c>
+      <c r="D1846" s="6">
+        <v>220.17749637023493</v>
+      </c>
+      <c r="E1846" s="6">
+        <v>111.09589973812209</v>
+      </c>
+      <c r="F1846" s="6">
+        <v>312.59252780809027</v>
+      </c>
+      <c r="H1846" s="6">
+        <v>3.0720863946794754</v>
+      </c>
+      <c r="J1846" s="6">
+        <v>19.595803519881208</v>
+      </c>
+      <c r="K1846" s="6">
+        <v>9.6029093929761338</v>
+      </c>
+      <c r="L1846" s="6">
+        <v>3.3923972931792101</v>
+      </c>
+      <c r="M1846" s="6">
+        <v>6.2978161257180751</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1847" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1847" s="5">
+        <v>42782</v>
+      </c>
+      <c r="C1847" s="6">
+        <v>1461.3264985345052</v>
+      </c>
+      <c r="D1847" s="6">
+        <v>174.77128743512009</v>
+      </c>
+      <c r="E1847" s="6">
+        <v>178.34964801014985</v>
+      </c>
+      <c r="F1847" s="6">
+        <v>1066.4123754018947</v>
+      </c>
+      <c r="H1847" s="6">
+        <v>3.2959221980901501</v>
+      </c>
+      <c r="J1847" s="6">
+        <v>23.709090856502076</v>
+      </c>
+      <c r="K1847" s="6">
+        <v>6.3108056623499547</v>
+      </c>
+      <c r="L1847" s="6">
+        <v>2.8952624134716176</v>
+      </c>
+      <c r="M1847" s="6">
+        <v>14.076951690472034</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1848" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1848" s="5">
+        <v>42823</v>
+      </c>
+      <c r="C1848" s="6">
+        <v>2403.0689570446621</v>
+      </c>
+      <c r="D1848" s="6">
+        <v>213.36250120743748</v>
+      </c>
+      <c r="E1848" s="6">
+        <v>374.45167415607779</v>
+      </c>
+      <c r="F1848" s="6">
+        <v>1743.5454553995373</v>
+      </c>
+      <c r="H1848" s="6">
+        <v>3.53149889119647</v>
+      </c>
+      <c r="J1848" s="6">
+        <v>39.860337611100931</v>
+      </c>
+      <c r="K1848" s="6">
+        <v>8.4993527625474705</v>
+      </c>
+      <c r="L1848" s="6">
+        <v>7.1485012354677036</v>
+      </c>
+      <c r="M1848" s="6">
+        <v>23.48790156776294</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1849" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1849" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1849" s="6">
+        <v>681.87821062337241</v>
+      </c>
+      <c r="D1849" s="6">
+        <v>95.218925479244291</v>
+      </c>
+      <c r="E1849" s="6">
+        <v>61.286504778831969</v>
+      </c>
+      <c r="F1849" s="6">
+        <v>511.55000968865943</v>
+      </c>
+      <c r="H1849" s="6">
+        <v>1.4014427147278294</v>
+      </c>
+      <c r="J1849" s="6">
+        <v>15.020227540498851</v>
+      </c>
+      <c r="K1849" s="6">
+        <v>3.7823384070525896</v>
+      </c>
+      <c r="L1849" s="6">
+        <v>1.5783080814195698</v>
+      </c>
+      <c r="M1849" s="6">
+        <v>9.4530850296042992</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1850" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1850" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1850" s="6">
+        <v>1381.5751094642342</v>
+      </c>
+      <c r="D1850" s="6">
+        <v>46.567466266577306</v>
+      </c>
+      <c r="E1850" s="6">
+        <v>31.129029957127766</v>
+      </c>
+      <c r="F1850" s="6">
+        <v>1176.3253976935853</v>
+      </c>
+      <c r="H1850" s="6">
+        <v>0.80282534610769873</v>
+      </c>
+      <c r="J1850" s="6">
+        <v>11.719485316451141</v>
+      </c>
+      <c r="K1850" s="6">
+        <v>1.627250576232268</v>
+      </c>
+      <c r="L1850" s="6">
+        <v>0.59383787944097377</v>
+      </c>
+      <c r="M1850" s="6">
+        <v>8.0357100188427761</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1851" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1851" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1851" s="6">
+        <v>847.94624161750085</v>
+      </c>
+      <c r="D1851" s="6">
+        <v>148.88112438444793</v>
+      </c>
+      <c r="E1851" s="6">
+        <v>111.36099218549619</v>
+      </c>
+      <c r="F1851" s="6">
+        <v>570.3606857283728</v>
+      </c>
+      <c r="H1851" s="6">
+        <v>2.0227850409085502</v>
+      </c>
+      <c r="J1851" s="6">
+        <v>22.714643914002878</v>
+      </c>
+      <c r="K1851" s="6">
+        <v>6.5895757832695789</v>
+      </c>
+      <c r="L1851" s="6">
+        <v>3.6557227822703311</v>
+      </c>
+      <c r="M1851" s="6">
+        <v>12.226693528798812</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1852" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1852" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1852" s="6">
+        <v>1956.551922816524</v>
+      </c>
+      <c r="D1852" s="6">
+        <v>74.729877628972005</v>
+      </c>
+      <c r="E1852" s="6">
+        <v>114.26047433383198</v>
+      </c>
+      <c r="F1852" s="6">
+        <v>1610.248353700898</v>
+      </c>
+      <c r="H1852" s="6">
+        <v>1.4702028861360221</v>
+      </c>
+      <c r="J1852" s="6">
+        <v>25.820952815401021</v>
+      </c>
+      <c r="K1852" s="6">
+        <v>3.0696327087092801</v>
+      </c>
+      <c r="L1852" s="6">
+        <v>2.3495420935318445</v>
+      </c>
+      <c r="M1852" s="6">
+        <v>18.037150043049795</v>
+      </c>
+    </row>
+    <row r="1853" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1853" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1853" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1853" s="6">
+        <v>885.99958701285516</v>
+      </c>
+      <c r="D1853" s="6">
+        <v>124.82504256689283</v>
+      </c>
+      <c r="E1853" s="6">
+        <v>97.828166093154749</v>
+      </c>
+      <c r="F1853" s="6">
+        <v>638.1935245421289</v>
+      </c>
+      <c r="H1853" s="6">
+        <v>1.3408652438258464</v>
+      </c>
+      <c r="J1853" s="6">
+        <v>20.332383310488968</v>
+      </c>
+      <c r="K1853" s="6">
+        <v>5.1134735093126116</v>
+      </c>
+      <c r="L1853" s="6">
+        <v>2.7829271563988476</v>
+      </c>
+      <c r="M1853" s="6">
+        <v>12.074110635102299</v>
+      </c>
+    </row>
+    <row r="1854" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1854" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1854" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1854" s="6">
+        <v>1992.0593196254981</v>
+      </c>
+      <c r="D1854" s="6">
+        <v>78.435728666638809</v>
+      </c>
+      <c r="E1854" s="6">
+        <v>94.308994065372431</v>
+      </c>
+      <c r="F1854" s="6">
+        <v>1655.994341736985</v>
+      </c>
+      <c r="H1854" s="6">
+        <v>1.5846651971483341</v>
+      </c>
+      <c r="J1854" s="6">
+        <v>29.231122305853621</v>
+      </c>
+      <c r="K1854" s="6">
+        <v>3.2849940511581139</v>
+      </c>
+      <c r="L1854" s="6">
+        <v>1.9833218551299143</v>
+      </c>
+      <c r="M1854" s="6">
+        <v>21.300519397681477</v>
+      </c>
+    </row>
+    <row r="1855" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1855" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1855" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1855" s="6">
+        <v>1492.8864233195363</v>
+      </c>
+      <c r="D1855" s="6">
+        <v>189.55522808468794</v>
+      </c>
+      <c r="E1855" s="6">
+        <v>156.79693333945022</v>
+      </c>
+      <c r="F1855" s="6">
+        <v>1120.6950820444436</v>
+      </c>
+      <c r="H1855" s="6">
+        <v>2.8615322711838762</v>
+      </c>
+      <c r="J1855" s="6">
+        <v>36.817041416039181</v>
+      </c>
+      <c r="K1855" s="6">
+        <v>7.812299714219475</v>
+      </c>
+      <c r="L1855" s="6">
+        <v>4.8961089523683903</v>
+      </c>
+      <c r="M1855" s="6">
+        <v>23.734370923972698</v>
+      </c>
+    </row>
+    <row r="1856" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1856" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1856" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1856" s="6">
+        <v>1879.518329138233</v>
+      </c>
+      <c r="D1856" s="6">
+        <v>89.224814476384026</v>
+      </c>
+      <c r="E1856" s="6">
+        <v>107.14305862114865</v>
+      </c>
+      <c r="F1856" s="6">
+        <v>1543.2073059143781</v>
+      </c>
+      <c r="H1856" s="6">
+        <v>1.6552696381610879</v>
+      </c>
+      <c r="J1856" s="6">
+        <v>33.552340598375721</v>
+      </c>
+      <c r="K1856" s="6">
+        <v>4.0414085667326116</v>
+      </c>
+      <c r="L1856" s="6">
+        <v>2.602606368166632</v>
+      </c>
+      <c r="M1856" s="6">
+        <v>24.290891649989263</v>
+      </c>
+    </row>
+    <row r="1857" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1857" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1857" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1857" s="6">
+        <v>681.87821062337241</v>
+      </c>
+      <c r="D1857" s="6">
+        <v>95.218925479244291</v>
+      </c>
+      <c r="E1857" s="6">
+        <v>61.286504778831969</v>
+      </c>
+      <c r="F1857" s="6">
+        <v>511.55000968865943</v>
+      </c>
+      <c r="H1857" s="6">
+        <v>1.4014427147278294</v>
+      </c>
+      <c r="J1857" s="6">
+        <v>15.020227540498851</v>
+      </c>
+      <c r="K1857" s="6">
+        <v>3.7823384070525896</v>
+      </c>
+      <c r="L1857" s="6">
+        <v>1.5783080814195698</v>
+      </c>
+      <c r="M1857" s="6">
+        <v>9.4530850296042992</v>
+      </c>
+    </row>
+    <row r="1858" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1858" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1858" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1858" s="6">
+        <v>1381.5751094642342</v>
+      </c>
+      <c r="D1858" s="6">
+        <v>46.567466266577306</v>
+      </c>
+      <c r="E1858" s="6">
+        <v>31.129029957127766</v>
+      </c>
+      <c r="F1858" s="6">
+        <v>1176.3253976935853</v>
+      </c>
+      <c r="H1858" s="6">
+        <v>0.80282534610769873</v>
+      </c>
+      <c r="J1858" s="6">
+        <v>11.719485316451141</v>
+      </c>
+      <c r="K1858" s="6">
+        <v>1.627250576232268</v>
+      </c>
+      <c r="L1858" s="6">
+        <v>0.59383787944097377</v>
+      </c>
+      <c r="M1858" s="6">
+        <v>8.0357100188427761</v>
+      </c>
+    </row>
+    <row r="1859" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1859" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1859" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1859" s="6">
+        <v>712.72633635804755</v>
+      </c>
+      <c r="D1859" s="6">
+        <v>152.87727441946362</v>
+      </c>
+      <c r="E1859" s="6">
+        <v>126.50202515192726</v>
+      </c>
+      <c r="F1859" s="6">
+        <v>412.96722162794532</v>
+      </c>
+      <c r="H1859" s="6">
+        <v>2.1273887738306279</v>
+      </c>
+      <c r="J1859" s="6">
+        <v>20.113563368925838</v>
+      </c>
+      <c r="K1859" s="6">
+        <v>6.7497802780803555</v>
+      </c>
+      <c r="L1859" s="6">
+        <v>4.0917759076576896</v>
+      </c>
+      <c r="M1859" s="6">
+        <v>8.9687883854077874</v>
+      </c>
+    </row>
+    <row r="1860" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1860" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1860" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1860" s="6">
+        <v>1670.4875014447364</v>
+      </c>
+      <c r="D1860" s="6">
+        <v>76.07319283408323</v>
+      </c>
+      <c r="E1860" s="6">
+        <v>80.729244737758435</v>
+      </c>
+      <c r="F1860" s="6">
+        <v>1407.0113438491949</v>
+      </c>
+      <c r="H1860" s="6">
+        <v>1.6295376416532594</v>
+      </c>
+      <c r="J1860" s="6">
+        <v>23.932132025517777</v>
+      </c>
+      <c r="K1860" s="6">
+        <v>3.1951027011275093</v>
+      </c>
+      <c r="L1860" s="6">
+        <v>1.759290004983266</v>
+      </c>
+      <c r="M1860" s="6">
+        <v>17.27797866126576</v>
+      </c>
+    </row>
+    <row r="1861" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1861" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1861" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1861" s="6">
+        <v>707.85961747354418</v>
+      </c>
+      <c r="D1861" s="6">
+        <v>142.34411183927384</v>
+      </c>
+      <c r="E1861" s="6">
+        <v>103.52370936494817</v>
+      </c>
+      <c r="F1861" s="6">
+        <v>439.41189546931383</v>
+      </c>
+      <c r="H1861" s="6">
+        <v>2.0640710099284214</v>
+      </c>
+      <c r="J1861" s="6">
+        <v>17.323347657893645</v>
+      </c>
+      <c r="K1861" s="6">
+        <v>5.7794976257824127</v>
+      </c>
+      <c r="L1861" s="6">
+        <v>2.813077736046417</v>
+      </c>
+      <c r="M1861" s="6">
+        <v>8.3933042220734766</v>
+      </c>
+    </row>
+    <row r="1862" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1862" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1862" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1862" s="6">
+        <v>1825.0523501722228</v>
+      </c>
+      <c r="D1862" s="6">
+        <v>88.010048047661215</v>
+      </c>
+      <c r="E1862" s="6">
+        <v>110.61218899314345</v>
+      </c>
+      <c r="F1862" s="6">
+        <v>1475.7045519160167</v>
+      </c>
+      <c r="H1862" s="6">
+        <v>1.7969387217713386</v>
+      </c>
+      <c r="J1862" s="6">
+        <v>30.789784790444447</v>
+      </c>
+      <c r="K1862" s="6">
+        <v>3.9915445592025813</v>
+      </c>
+      <c r="L1862" s="6">
+        <v>2.5881264717496846</v>
+      </c>
+      <c r="M1862" s="6">
+        <v>21.293171726724879</v>
+      </c>
+    </row>
+    <row r="1863" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1863" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1863" s="5">
+        <v>42762</v>
+      </c>
+      <c r="C1863" s="6">
+        <v>539.34040214610911</v>
+      </c>
+      <c r="D1863" s="6">
+        <v>111.96606673704063</v>
+      </c>
+      <c r="E1863" s="6">
+        <v>66.729438244220788</v>
+      </c>
+      <c r="F1863" s="6">
+        <v>344.5922776246469</v>
+      </c>
+      <c r="H1863" s="6">
+        <v>1.5375611290422588</v>
+      </c>
+      <c r="J1863" s="6">
+        <v>13.238524005465019</v>
+      </c>
+      <c r="K1863" s="6">
+        <v>4.6348866198113949</v>
+      </c>
+      <c r="L1863" s="6">
+        <v>1.9027316732224715</v>
+      </c>
+      <c r="M1863" s="6">
+        <v>6.483058453388006</v>
+      </c>
+    </row>
+    <row r="1864" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1864" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1864" s="5">
+        <v>42846</v>
+      </c>
+      <c r="C1864" s="6">
+        <v>1800.3891531985441</v>
+      </c>
+      <c r="D1864" s="6">
+        <v>112.7853798864968</v>
+      </c>
+      <c r="E1864" s="6">
+        <v>110.58632276445823</v>
+      </c>
+      <c r="F1864" s="6">
+        <v>1425.9338317369227</v>
+      </c>
+      <c r="H1864" s="6">
+        <v>2.3968629402659043</v>
+      </c>
+      <c r="J1864" s="6">
+        <v>37.156930641423941</v>
+      </c>
+      <c r="K1864" s="6">
+        <v>5.0622763288979762</v>
+      </c>
+      <c r="L1864" s="6">
+        <v>2.905646378375967</v>
+      </c>
+      <c r="M1864" s="6">
+        <v>26.387704332214213</v>
+      </c>
+    </row>
+    <row r="1865" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1865" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1865" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1865" s="6">
+        <v>890.11353683413267</v>
+      </c>
+      <c r="D1865" s="6">
+        <v>237.99004523425901</v>
+      </c>
+      <c r="E1865" s="6">
+        <v>183.51080333808471</v>
+      </c>
+      <c r="F1865" s="6">
+        <v>442.13769888061023</v>
+      </c>
+      <c r="H1865" s="6">
+        <v>4.3461121578688386</v>
+      </c>
+      <c r="J1865" s="6">
+        <v>23.097646667060356</v>
+      </c>
+      <c r="K1865" s="6">
+        <v>10.051032623971532</v>
+      </c>
+      <c r="L1865" s="6">
+        <v>4.4543899051463125</v>
+      </c>
+      <c r="M1865" s="6">
+        <v>8.1216822364772572</v>
+      </c>
+    </row>
+    <row r="1866" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1866" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1866" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1866" s="6">
+        <v>1541.7600789952994</v>
+      </c>
+      <c r="D1866" s="6">
+        <v>206.96432662713087</v>
+      </c>
+      <c r="E1866" s="6">
+        <v>186.65299508465432</v>
+      </c>
+      <c r="F1866" s="6">
+        <v>1093.6216288602732</v>
+      </c>
+      <c r="H1866" s="6">
+        <v>3.5902577536821809</v>
+      </c>
+      <c r="J1866" s="6">
+        <v>27.355796681741463</v>
+      </c>
+      <c r="K1866" s="6">
+        <v>7.2693550960416307</v>
+      </c>
+      <c r="L1866" s="6">
+        <v>3.4370065082475469</v>
+      </c>
+      <c r="M1866" s="6">
+        <v>15.915895355434984</v>
+      </c>
+    </row>
+    <row r="1867" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1867" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1867" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1867" s="6">
+        <v>2492.0020497287496</v>
+      </c>
+      <c r="D1867" s="6">
+        <v>94.605118670221117</v>
+      </c>
+      <c r="E1867" s="6">
+        <v>138.3963512539255</v>
+      </c>
+      <c r="F1867" s="6">
+        <v>2029.5409933438073</v>
+      </c>
+      <c r="H1867" s="6">
+        <v>1.5869055135073875</v>
+      </c>
+      <c r="J1867" s="6">
+        <v>45.165542631233066</v>
+      </c>
+      <c r="K1867" s="6">
+        <v>4.3968506840692463</v>
+      </c>
+      <c r="L1867" s="6">
+        <v>3.6686568898659551</v>
+      </c>
+      <c r="M1867" s="6">
+        <v>31.94275855087367</v>
+      </c>
+    </row>
+    <row r="1868" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1868" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1868" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1868" s="6">
+        <v>1131.8339196680056</v>
+      </c>
+      <c r="D1868" s="6">
+        <v>343.74012160626205</v>
+      </c>
+      <c r="E1868" s="6">
+        <v>207.90371992358078</v>
+      </c>
+      <c r="F1868" s="6">
+        <v>558.12080016600623</v>
+      </c>
+      <c r="H1868" s="6">
+        <v>6.1274149995430269</v>
+      </c>
+      <c r="J1868" s="6">
+        <v>31.004390325455567</v>
+      </c>
+      <c r="K1868" s="6">
+        <v>14.377306388093492</v>
+      </c>
+      <c r="L1868" s="6">
+        <v>5.2397236692916476</v>
+      </c>
+      <c r="M1868" s="6">
+        <v>10.975955364241019</v>
+      </c>
+    </row>
+    <row r="1869" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1869" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1869" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1869" s="6">
+        <v>1862.1562382203035</v>
+      </c>
+      <c r="D1869" s="6">
+        <v>193.06565953738954</v>
+      </c>
+      <c r="E1869" s="6">
+        <v>178.37989501148269</v>
+      </c>
+      <c r="F1869" s="6">
+        <v>1405.3661509414305</v>
+      </c>
+      <c r="H1869" s="6">
+        <v>3.0851328067273514</v>
+      </c>
+      <c r="J1869" s="6">
+        <v>32.485814503426766</v>
+      </c>
+      <c r="K1869" s="6">
+        <v>7.056283653433189</v>
+      </c>
+      <c r="L1869" s="6">
+        <v>3.5046504544590227</v>
+      </c>
+      <c r="M1869" s="6">
+        <v>20.534949915165093</v>
+      </c>
+    </row>
+    <row r="1870" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1870" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1870" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1870" s="6">
+        <v>2913.7489075137155</v>
+      </c>
+      <c r="D1870" s="6">
+        <v>116.19915164191279</v>
+      </c>
+      <c r="E1870" s="6">
+        <v>144.36460023246519</v>
+      </c>
+      <c r="F1870" s="6">
+        <v>2410.7244677190679</v>
+      </c>
+      <c r="H1870" s="6">
+        <v>1.9485796900047747</v>
+      </c>
+      <c r="J1870" s="6">
+        <v>34.364496335957035</v>
+      </c>
+      <c r="K1870" s="6">
+        <v>4.5611412827240194</v>
+      </c>
+      <c r="L1870" s="6">
+        <v>2.4244548114796669</v>
+      </c>
+      <c r="M1870" s="6">
+        <v>23.661446051271295</v>
+      </c>
+    </row>
+    <row r="1871" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1871" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1871" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1871" s="6">
+        <v>955.76949429995875</v>
+      </c>
+      <c r="D1871" s="6">
+        <v>262.41488782020508</v>
+      </c>
+      <c r="E1871" s="6">
+        <v>203.24747844945017</v>
+      </c>
+      <c r="F1871" s="6">
+        <v>459.52790125776983</v>
+      </c>
+      <c r="H1871" s="6">
+        <v>4.8283834123014566</v>
+      </c>
+      <c r="J1871" s="6">
+        <v>25.224401624111813</v>
+      </c>
+      <c r="K1871" s="6">
+        <v>11.012992948467202</v>
+      </c>
+      <c r="L1871" s="6">
+        <v>5.0027225701201381</v>
+      </c>
+      <c r="M1871" s="6">
+        <v>8.6028884953545184</v>
+      </c>
+    </row>
+    <row r="1872" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1872" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1872" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1872" s="6">
+        <v>1509.0530276534021</v>
+      </c>
+      <c r="D1872" s="6">
+        <v>203.13644352985159</v>
+      </c>
+      <c r="E1872" s="6">
+        <v>149.47383237188859</v>
+      </c>
+      <c r="F1872" s="6">
+        <v>1093.9052031074505</v>
+      </c>
+      <c r="H1872" s="6">
+        <v>3.2960011999443317</v>
+      </c>
+      <c r="J1872" s="6">
+        <v>29.827432380918729</v>
+      </c>
+      <c r="K1872" s="6">
+        <v>7.6974915051420725</v>
+      </c>
+      <c r="L1872" s="6">
+        <v>3.0368517553735241</v>
+      </c>
+      <c r="M1872" s="6">
+        <v>18.262874185525504</v>
+      </c>
+    </row>
+    <row r="1873" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1873" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1873" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1873" s="6">
+        <v>2422.1930640542023</v>
+      </c>
+      <c r="D1873" s="6">
+        <v>127.64058294911874</v>
+      </c>
+      <c r="E1873" s="6">
+        <v>178.62729153157352</v>
+      </c>
+      <c r="F1873" s="6">
+        <v>1840.852718718538</v>
+      </c>
+      <c r="H1873" s="6">
+        <v>2.1624406830232279</v>
+      </c>
+      <c r="J1873" s="6">
+        <v>44.180451317382342</v>
+      </c>
+      <c r="K1873" s="6">
+        <v>6.0672897924285767</v>
+      </c>
+      <c r="L1873" s="6">
+        <v>4.1663128118627535</v>
+      </c>
+      <c r="M1873" s="6">
+        <v>28.275159479419749</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1874" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1874" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1874" s="6">
+        <v>1284.4577734161321</v>
+      </c>
+      <c r="D1874" s="6">
+        <v>305.31243983652905</v>
+      </c>
+      <c r="E1874" s="6">
+        <v>214.57974148609122</v>
+      </c>
+      <c r="F1874" s="6">
+        <v>733.96009279667146</v>
+      </c>
+      <c r="H1874" s="6">
+        <v>5.096039097896214</v>
+      </c>
+      <c r="J1874" s="6">
+        <v>34.028335267386659</v>
+      </c>
+      <c r="K1874" s="6">
+        <v>13.283342770513325</v>
+      </c>
+      <c r="L1874" s="6">
+        <v>5.5389055469615007</v>
+      </c>
+      <c r="M1874" s="6">
+        <v>14.606001434058598</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1875" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1875" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1875" s="6">
+        <v>1690.4615574404957</v>
+      </c>
+      <c r="D1875" s="6">
+        <v>220.22088893605709</v>
+      </c>
+      <c r="E1875" s="6">
+        <v>184.66302449094439</v>
+      </c>
+      <c r="F1875" s="6">
+        <v>1209.2414803839952</v>
+      </c>
+      <c r="H1875" s="6">
+        <v>3.4612298043809528</v>
+      </c>
+      <c r="J1875" s="6">
+        <v>36.227204253136307</v>
+      </c>
+      <c r="K1875" s="6">
+        <v>8.8833928254860943</v>
+      </c>
+      <c r="L1875" s="6">
+        <v>4.2382772069086476</v>
+      </c>
+      <c r="M1875" s="6">
+        <v>21.529927643538326</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1876" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1876" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1876" s="6">
+        <v>2426.4229815919766</v>
+      </c>
+      <c r="D1876" s="6">
+        <v>80.062430088094331</v>
+      </c>
+      <c r="E1876" s="6">
+        <v>117.48611614289185</v>
+      </c>
+      <c r="F1876" s="6">
+        <v>1990.969179489987</v>
+      </c>
+      <c r="H1876" s="6">
+        <v>1.3588196548459341</v>
+      </c>
+      <c r="J1876" s="6">
+        <v>44.950081293362274</v>
+      </c>
+      <c r="K1876" s="6">
+        <v>3.9764624385342211</v>
+      </c>
+      <c r="L1876" s="6">
+        <v>2.8986037165310323</v>
+      </c>
+      <c r="M1876" s="6">
+        <v>33.210685137176284</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1877" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1877" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1877" s="6">
+        <v>824.36990077351413</v>
+      </c>
+      <c r="D1877" s="6">
+        <v>236.94522823410489</v>
+      </c>
+      <c r="E1877" s="6">
+        <v>150.76637096115365</v>
+      </c>
+      <c r="F1877" s="6">
+        <v>412.90432079217271</v>
+      </c>
+      <c r="H1877" s="6">
+        <v>4.3461121578688386</v>
+      </c>
+      <c r="J1877" s="6">
+        <v>21.645403498795634</v>
+      </c>
+      <c r="K1877" s="6">
+        <v>10.129185382706577</v>
+      </c>
+      <c r="L1877" s="6">
+        <v>3.9008615598426788</v>
+      </c>
+      <c r="M1877" s="6">
+        <v>7.4550558232493414</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1878" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1878" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1878" s="6">
+        <v>1892.8745684283167</v>
+      </c>
+      <c r="D1878" s="6">
+        <v>219.22914893118437</v>
+      </c>
+      <c r="E1878" s="6">
+        <v>166.26087018251249</v>
+      </c>
+      <c r="F1878" s="6">
+        <v>1226.4273006933465</v>
+      </c>
+      <c r="H1878" s="6">
+        <v>3.5902577536821809</v>
+      </c>
+      <c r="J1878" s="6">
+        <v>38.787840452377004</v>
+      </c>
+      <c r="K1878" s="6">
+        <v>7.8833463869178626</v>
+      </c>
+      <c r="L1878" s="6">
+        <v>3.6676125162183091</v>
+      </c>
+      <c r="M1878" s="6">
+        <v>22.712793656233124</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1879" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1879" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1879" s="6">
+        <v>2472.8387391410915</v>
+      </c>
+      <c r="D1879" s="6">
+        <v>111.70063952952971</v>
+      </c>
+      <c r="E1879" s="6">
+        <v>183.38726659197897</v>
+      </c>
+      <c r="F1879" s="6">
+        <v>1950.6503566423028</v>
+      </c>
+      <c r="H1879" s="6">
+        <v>1.5869055135073875</v>
+      </c>
+      <c r="J1879" s="6">
+        <v>44.847841322450058</v>
+      </c>
+      <c r="K1879" s="6">
+        <v>5.062625920868447</v>
+      </c>
+      <c r="L1879" s="6">
+        <v>4.0154297409832758</v>
+      </c>
+      <c r="M1879" s="6">
+        <v>31.299211257308411</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1880" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1880" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1880" s="6">
+        <v>824.36990077351413</v>
+      </c>
+      <c r="D1880" s="6">
+        <v>236.94522823410489</v>
+      </c>
+      <c r="E1880" s="6">
+        <v>150.76637096115365</v>
+      </c>
+      <c r="F1880" s="6">
+        <v>412.90432079217271</v>
+      </c>
+      <c r="H1880" s="6">
+        <v>4.7177696726371696</v>
+      </c>
+      <c r="J1880" s="6">
+        <v>21.645403498795634</v>
+      </c>
+      <c r="K1880" s="6">
+        <v>10.129185382706577</v>
+      </c>
+      <c r="L1880" s="6">
+        <v>3.9008615598426788</v>
+      </c>
+      <c r="M1880" s="6">
+        <v>7.4550558232493414</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1881" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1881" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1881" s="6">
+        <v>1892.8745684283167</v>
+      </c>
+      <c r="D1881" s="6">
+        <v>219.22914893118437</v>
+      </c>
+      <c r="E1881" s="6">
+        <v>166.26087018251249</v>
+      </c>
+      <c r="F1881" s="6">
+        <v>1226.4273006933465</v>
+      </c>
+      <c r="H1881" s="6">
+        <v>3.330851468445724</v>
+      </c>
+      <c r="J1881" s="6">
+        <v>38.787840452377004</v>
+      </c>
+      <c r="K1881" s="6">
+        <v>7.8833463869178626</v>
+      </c>
+      <c r="L1881" s="6">
+        <v>3.6676125162183091</v>
+      </c>
+      <c r="M1881" s="6">
+        <v>22.712793656233124</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1882" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1882" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1882" s="6">
+        <v>2472.8387391410915</v>
+      </c>
+      <c r="D1882" s="6">
+        <v>111.70063952952971</v>
+      </c>
+      <c r="E1882" s="6">
+        <v>183.38726659197897</v>
+      </c>
+      <c r="F1882" s="6">
+        <v>1950.6503566423028</v>
+      </c>
+      <c r="H1882" s="6">
+        <v>1.9538079338494221</v>
+      </c>
+      <c r="J1882" s="6">
+        <v>44.847841322450058</v>
+      </c>
+      <c r="K1882" s="6">
+        <v>5.062625920868447</v>
+      </c>
+      <c r="L1882" s="6">
+        <v>4.0154297409832758</v>
+      </c>
+      <c r="M1882" s="6">
+        <v>31.299211257308411</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1883" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1883" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1883" s="6">
+        <v>1038.7860862295918</v>
+      </c>
+      <c r="D1883" s="6">
+        <v>303.04553421210392</v>
+      </c>
+      <c r="E1883" s="6">
+        <v>190.85701510123411</v>
+      </c>
+      <c r="F1883" s="6">
+        <v>515.91153677391162</v>
+      </c>
+      <c r="H1883" s="6">
+        <v>5.3207188793133193</v>
+      </c>
+      <c r="J1883" s="6">
+        <v>27.914927650353953</v>
+      </c>
+      <c r="K1883" s="6">
+        <v>12.997168025255338</v>
+      </c>
+      <c r="L1883" s="6">
+        <v>4.8013141405200352</v>
+      </c>
+      <c r="M1883" s="6">
+        <v>9.5760633166781997</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1884" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1884" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1884" s="6">
+        <v>1862.4235998390357</v>
+      </c>
+      <c r="D1884" s="6">
+        <v>194.41410891387841</v>
+      </c>
+      <c r="E1884" s="6">
+        <v>161.71004414913597</v>
+      </c>
+      <c r="F1884" s="6">
+        <v>1445.1450094825564</v>
+      </c>
+      <c r="H1884" s="6">
+        <v>3.1833158318551473</v>
+      </c>
+      <c r="J1884" s="6">
+        <v>32.925589254485807</v>
+      </c>
+      <c r="K1884" s="6">
+        <v>7.1252021103030172</v>
+      </c>
+      <c r="L1884" s="6">
+        <v>3.2537773739116274</v>
+      </c>
+      <c r="M1884" s="6">
+        <v>21.719240815906012</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1885" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1885" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1885" s="6">
+        <v>2756.7779133747185</v>
+      </c>
+      <c r="D1885" s="6">
+        <v>135.76177095866635</v>
+      </c>
+      <c r="E1885" s="6">
+        <v>217.05646184127835</v>
+      </c>
+      <c r="F1885" s="6">
+        <v>2176.16178719555</v>
+      </c>
+      <c r="H1885" s="6">
+        <v>2.7180941867477189</v>
+      </c>
+      <c r="J1885" s="6">
+        <v>53.623670557819835</v>
+      </c>
+      <c r="K1885" s="6">
+        <v>6.6178815864118334</v>
+      </c>
+      <c r="L1885" s="6">
+        <v>5.4140185788558224</v>
+      </c>
+      <c r="M1885" s="6">
+        <v>37.066871014704574</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1886" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1886" s="5">
+        <v>42746</v>
+      </c>
+      <c r="C1886" s="6">
+        <v>969.15061515478692</v>
+      </c>
+      <c r="D1886" s="6">
+        <v>287.4432673925379</v>
+      </c>
+      <c r="E1886" s="6">
+        <v>198.23643411650781</v>
+      </c>
+      <c r="F1886" s="6">
+        <v>453.66423145495099</v>
+      </c>
+      <c r="H1886" s="6">
+        <v>5.5916132361715158</v>
+      </c>
+      <c r="J1886" s="6">
+        <v>26.101120964484796</v>
+      </c>
+      <c r="K1886" s="6">
+        <v>11.888305336690173</v>
+      </c>
+      <c r="L1886" s="6">
+        <v>4.8052314899553865</v>
+      </c>
+      <c r="M1886" s="6">
+        <v>8.8395167590497703</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1887" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1887" s="5">
+        <v>42789</v>
+      </c>
+      <c r="C1887" s="6">
+        <v>1825.5231870143286</v>
+      </c>
+      <c r="D1887" s="6">
+        <v>193.23534300079484</v>
+      </c>
+      <c r="E1887" s="6">
+        <v>197.81039106735582</v>
+      </c>
+      <c r="F1887" s="6">
+        <v>1371.3941623006635</v>
+      </c>
+      <c r="H1887" s="6">
+        <v>3.4451361131405354</v>
+      </c>
+      <c r="J1887" s="6">
+        <v>32.109770347583144</v>
+      </c>
+      <c r="K1887" s="6">
+        <v>7.4622688912374286</v>
+      </c>
+      <c r="L1887" s="6">
+        <v>3.8467788533112914</v>
+      </c>
+      <c r="M1887" s="6">
+        <v>19.805318047523606</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1888" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1888" s="5">
+        <v>42858</v>
+      </c>
+      <c r="C1888" s="6">
+        <v>2561.594491663554</v>
+      </c>
+      <c r="D1888" s="6">
+        <v>139.59956045160641</v>
+      </c>
+      <c r="E1888" s="6">
+        <v>134.81684747544747</v>
+      </c>
+      <c r="F1888" s="6">
+        <v>2065.1676689085298</v>
+      </c>
+      <c r="H1888" s="6">
+        <v>2.3725024198832845</v>
+      </c>
+      <c r="J1888" s="6">
+        <v>46.968801625550938</v>
+      </c>
+      <c r="K1888" s="6">
+        <v>5.9963388375400051</v>
+      </c>
+      <c r="L1888" s="6">
+        <v>3.0323310024725987</v>
+      </c>
+      <c r="M1888" s="6">
+        <v>33.753374659900672</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>